<commit_message>
Changes to document and new test results in the protocol
</commit_message>
<xml_diff>
--- a/QualiMasterApplication/documentation/Testing Protocol.xlsx
+++ b/QualiMasterApplication/documentation/Testing Protocol.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14250" windowHeight="6900"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13290" windowHeight="9285"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="57">
   <si>
     <t>Result</t>
   </si>
@@ -173,6 +173,21 @@
   </si>
   <si>
     <t>Roman: 0.8.5 win 64-bit (2016-01-11), Windows 7 64-bit, Java jdk1.8.0_66 64-bit</t>
+  </si>
+  <si>
+    <t>Roman: 0.8.5 win 64-bit (2016-01-12), Windows 7 64-bit, Java jdk1.8.0_66 64-bit</t>
+  </si>
+  <si>
+    <t>Selection is possible, but the editor is not set dirty. As workaround make some other change and then it is possible to save.</t>
+  </si>
+  <si>
+    <t>For GP Machines name in the view changes only after restarting app; attribute fileds in the UI of a new added Data Management and Algorithms are smaller;</t>
+  </si>
+  <si>
+    <t>From sink only output, from source input; when copying it does not add but replaces all fields you already have;</t>
+  </si>
+  <si>
+    <t>Algorithm Family do not have constraints in UI (changed document); in Pipeline Editor possible to add constraint for all elements(after adding click on the diagram space to set editor dirty); in Pipeline editorconstraints not check for syntax (name &gt; 1 can be added)</t>
   </si>
 </sst>
 </file>
@@ -216,7 +231,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -224,46 +239,168 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -560,374 +697,560 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="49.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3"/>
-    <col min="4" max="4" width="65" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="11.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="49.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="65" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="58.28515625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="3"/>
-      <c r="C1" s="12" t="s">
+    <row r="1" spans="1:8" ht="15" customHeight="1">
+      <c r="A1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="25"/>
+      <c r="H1" s="26"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="15" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="4">
+      <c r="F2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="H2" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="18" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="4">
+      <c r="F3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="17"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="4">
+      <c r="C4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30">
-      <c r="A6" s="4">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="C5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" ht="30">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="4">
+      <c r="F6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30">
-      <c r="A8" s="4">
+      <c r="C7" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" ht="30">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="18" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="4">
+      <c r="F8" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" ht="48.75" customHeight="1">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="4">
+      <c r="F9" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45">
-      <c r="A11" s="4">
+      <c r="C10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="45">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="45">
-      <c r="A12" s="4">
+      <c r="C11" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="45">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="C12" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="45">
-      <c r="A13" s="4">
+      <c r="F12" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" ht="45">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="45">
-      <c r="A14" s="4">
+      <c r="C13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="17"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" ht="45">
+      <c r="A14" s="3">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="45">
-      <c r="A15" s="4">
+      <c r="C14" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="17"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" ht="45">
+      <c r="A15" s="3">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30">
-      <c r="A16" s="4">
+      <c r="C15" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" ht="30">
+      <c r="A16" s="3">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="C16" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="4">
+      <c r="F16" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="3">
         <v>15</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="4">
+      <c r="C17" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="17"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="3">
         <v>16</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="4">
+      <c r="C18" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="3">
         <v>17</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30">
-      <c r="A20" s="4">
+      <c r="C19" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="17"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="17"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" ht="75">
+      <c r="A20" s="3">
         <v>18</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="17" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="4">
+      <c r="E20" s="4"/>
+      <c r="F20" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="3">
         <v>19</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="4">
+      <c r="C21" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="17"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="3">
         <v>20</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="4">
+      <c r="C22" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="17"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="3">
         <v>21</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="30">
+      <c r="C23" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="17"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" ht="30">
       <c r="A24" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="C24" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="18" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="30">
+      <c r="F24" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="17"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" ht="30">
       <c r="A25" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30">
+      <c r="C25" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="17"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" ht="30">
       <c r="A26" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="C26" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="4">
+      <c r="F26" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="17"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A27" s="7">
         <v>22</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="C27" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="23"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="23"/>
+      <c r="H27" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Test protocol for Linux tool
</commit_message>
<xml_diff>
--- a/QualiMasterApplication/documentation/Testing Protocol.xlsx
+++ b/QualiMasterApplication/documentation/Testing Protocol.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="13290" windowHeight="9285"/>
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="68">
   <si>
     <t>Result</t>
   </si>
@@ -188,13 +187,52 @@
   </si>
   <si>
     <t>Algorithm Family do not have constraints in UI (changed document); in Pipeline Editor possible to add constraint for all elements(after adding click on the diagram space to set editor dirty); in Pipeline editorconstraints not check for syntax (name &gt; 1 can be added)</t>
+  </si>
+  <si>
+    <t>Sascha: 0.8.5 Linux 64-bit (2016-01-12), Ubuntu 14.04.1 64-bit, Java 1.7.0_65 64-bit</t>
+  </si>
+  <si>
+    <t>pass/?</t>
+  </si>
+  <si>
+    <t>After testing "yes", I'm not able to test "no" as it is only asking the first time. But changes can be reverted using the revert all button.</t>
+  </si>
+  <si>
+    <t>Ctrl + Shift + S works also for saving all, but it does not ask. However, this is not part of the testing protocol.</t>
+  </si>
+  <si>
+    <t>First time when I clicked on browse the artifact tree did not opened (tested on Random Sink), afterwards it opened every time.
+OK works
+Cancel/Close button is missing, I need to click on X.
+Refresh brings me to the root of the tree and closes all member. Thus, I'm lost and I do not know how to navigate back to the qualimaster artifacts.</t>
+  </si>
+  <si>
+    <t>error in test specification</t>
+  </si>
+  <si>
+    <t>Revert|all does not exist in scenario 2 (local mode)</t>
+  </si>
+  <si>
+    <t>Deleted element, and directly re-added a new element. This new element is shown inside the TreeView as "ports" independently of ist real name. The name will be displayed corectly after a restart of the tool.</t>
+  </si>
+  <si>
+    <t>Unclear what "connect Family Element to remaining pipeline" means. Which part of the pipeline?</t>
+  </si>
+  <si>
+    <t>Pipeline editor does not work, if I click into the properties editor, the cell will only be black
+I do not find the configurable constraints inside the other editors.
+Needed help from Roman to find Constraint editor in ohter editors (only available for sources).
+Added constraint "name.size() &gt; 100" to RandomSource, saved, and pressed validate -&gt; No error detected.</t>
+  </si>
+  <si>
+    <t>role is not decorated, everything else is decorated correctly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -403,19 +441,130 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>35547</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>438149</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>409575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Grafik 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19571322" y="2085975"/>
+          <a:ext cx="3450602" cy="4229100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>15156</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>371476</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Grafik 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19550931" y="7029450"/>
+          <a:ext cx="7061920" cy="4400550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -453,7 +602,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -487,6 +636,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -521,9 +671,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -696,14 +847,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="49.140625" style="1" customWidth="1"/>
@@ -712,10 +863,13 @@
     <col min="5" max="5" width="15" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="58.28515625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="14.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="52.140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
       <c r="C1" s="24" t="s">
@@ -728,8 +882,13 @@
       </c>
       <c r="G1" s="25"/>
       <c r="H1" s="26"/>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
@@ -754,8 +913,17 @@
       <c r="H2" s="15" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="30">
+      <c r="I2" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="33" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -776,8 +944,15 @@
       </c>
       <c r="G3" s="17"/>
       <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="28"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -794,8 +969,13 @@
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -812,8 +992,13 @@
       </c>
       <c r="G5" s="17"/>
       <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" ht="30">
+      <c r="I5" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+    </row>
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -834,8 +1019,15 @@
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" s="28"/>
+    </row>
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -852,8 +1044,15 @@
       </c>
       <c r="G7" s="17"/>
       <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" ht="30">
+      <c r="I7" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7" s="28"/>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -874,8 +1073,15 @@
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" ht="48.75" customHeight="1">
+      <c r="I8" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" s="28"/>
+    </row>
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -898,8 +1104,11 @@
         <v>53</v>
       </c>
       <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" s="35"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="28"/>
+    </row>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -916,8 +1125,15 @@
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" ht="45">
+      <c r="I10" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="J10" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" s="28"/>
+    </row>
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -934,8 +1150,13 @@
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" ht="45">
+      <c r="I11" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+    </row>
+    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -958,8 +1179,13 @@
         <v>54</v>
       </c>
       <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" ht="45">
+      <c r="I12" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+    </row>
+    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -976,8 +1202,13 @@
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" ht="45">
+      <c r="I13" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+    </row>
+    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -994,8 +1225,15 @@
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" ht="45">
+      <c r="I14" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" s="28"/>
+    </row>
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1012,8 +1250,13 @@
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" ht="30">
+      <c r="I15" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+    </row>
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1036,8 +1279,13 @@
         <v>55</v>
       </c>
       <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -1054,8 +1302,12 @@
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17" s="28"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -1072,8 +1324,12 @@
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J18" s="28"/>
+    </row>
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -1090,8 +1346,14 @@
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" ht="75">
+      <c r="I19" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -1112,8 +1374,14 @@
         <v>56</v>
       </c>
       <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" s="30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1130,8 +1398,12 @@
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" s="28"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -1148,8 +1420,12 @@
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" s="28"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -1166,8 +1442,12 @@
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" ht="30">
+      <c r="I23" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J23" s="28"/>
+    </row>
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>30</v>
       </c>
@@ -1188,8 +1468,14 @@
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="1:8" ht="30">
+      <c r="I24" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="J24" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>31</v>
       </c>
@@ -1206,8 +1492,12 @@
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:8" ht="30">
+      <c r="I25" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J25" s="28"/>
+    </row>
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>32</v>
       </c>
@@ -1228,8 +1518,12 @@
       </c>
       <c r="G26" s="17"/>
       <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1">
+      <c r="I26" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26" s="28"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>22</v>
       </c>
@@ -1246,36 +1540,44 @@
       </c>
       <c r="G27" s="23"/>
       <c r="H27" s="8"/>
+      <c r="I27" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
7 test case works
</commit_message>
<xml_diff>
--- a/QualiMasterApplication/documentation/Testing Protocol.xlsx
+++ b/QualiMasterApplication/documentation/Testing Protocol.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="13290" windowHeight="9285"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -177,9 +178,6 @@
     <t>Roman: 0.8.5 win 64-bit (2016-01-12), Windows 7 64-bit, Java jdk1.8.0_66 64-bit</t>
   </si>
   <si>
-    <t>Selection is possible, but the editor is not set dirty. As workaround make some other change and then it is possible to save.</t>
-  </si>
-  <si>
     <t>For GP Machines name in the view changes only after restarting app; attribute fileds in the UI of a new added Data Management and Algorithms are smaller;</t>
   </si>
   <si>
@@ -227,12 +225,15 @@
   <si>
     <t>role is not decorated, everything else is decorated correctly</t>
   </si>
+  <si>
+    <t>Selection is possible, but the editor is set dirty after clicking on pipeline editor fieldthen it is possible to save.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,7 +250,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,6 +266,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -361,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -431,18 +438,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -460,15 +455,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -492,8 +502,8 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>438149</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>409575</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -503,7 +513,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -541,7 +551,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -562,9 +572,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -602,7 +612,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -636,7 +646,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -671,10 +680,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -847,14 +855,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="49.140625" style="1" customWidth="1"/>
@@ -869,26 +877,26 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="24" t="s">
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G1" s="31"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
@@ -913,17 +921,17 @@
       <c r="H2" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="I2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="29" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="30">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -944,15 +952,15 @@
       </c>
       <c r="G3" s="17"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="30" t="s">
+      <c r="I3" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="28"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K3" s="24"/>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -969,13 +977,13 @@
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I4" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -992,13 +1000,13 @@
       </c>
       <c r="G5" s="17"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-    </row>
-    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="I5" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+    </row>
+    <row r="6" spans="1:11" ht="45">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1019,15 +1027,15 @@
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="32" t="s">
+      <c r="I6" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="J6" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="K6" s="28"/>
-    </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="K6" s="24"/>
+    </row>
+    <row r="7" spans="1:11" ht="30">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1044,15 +1052,15 @@
       </c>
       <c r="G7" s="17"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J7" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="K7" s="28"/>
-    </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="I7" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="K7" s="24"/>
+    </row>
+    <row r="8" spans="1:11" ht="30">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1077,11 +1085,11 @@
         <v>27</v>
       </c>
       <c r="J8" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="K8" s="28"/>
-    </row>
-    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="K8" s="24"/>
+    </row>
+    <row r="9" spans="1:11" ht="30">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1097,18 +1105,18 @@
       <c r="E9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="20" t="s">
-        <v>40</v>
+      <c r="F9" s="36" t="s">
+        <v>4</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="35"/>
       <c r="J9" s="34"/>
-      <c r="K9" s="28"/>
-    </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="K9" s="24"/>
+    </row>
+    <row r="10" spans="1:11" ht="30">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1125,15 +1133,15 @@
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="31" t="s">
+      <c r="I10" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="J10" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="K10" s="28"/>
-    </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="K10" s="24"/>
+    </row>
+    <row r="11" spans="1:11" ht="45">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1150,13 +1158,13 @@
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-    </row>
-    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="I11" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+    </row>
+    <row r="12" spans="1:11" ht="45">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1176,16 +1184,16 @@
         <v>4</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H12" s="4"/>
-      <c r="I12" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-    </row>
-    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="I12" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+    </row>
+    <row r="13" spans="1:11" ht="45">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1202,13 +1210,13 @@
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-    </row>
-    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="I13" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+    </row>
+    <row r="14" spans="1:11" ht="60">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1225,15 +1233,15 @@
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="31" t="s">
+      <c r="I14" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="J14" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="K14" s="28"/>
-    </row>
-    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="J14" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="K14" s="24"/>
+    </row>
+    <row r="15" spans="1:11" ht="45">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1250,13 +1258,13 @@
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-    </row>
-    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="I15" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+    </row>
+    <row r="16" spans="1:11" ht="30">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1276,16 +1284,16 @@
         <v>4</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H16" s="4"/>
-      <c r="I16" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -1302,12 +1310,12 @@
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J17" s="28"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17" s="24"/>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -1324,12 +1332,12 @@
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J18" s="28"/>
-    </row>
-    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="I18" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J18" s="24"/>
+    </row>
+    <row r="19" spans="1:10" ht="30">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -1346,14 +1354,14 @@
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J19" s="30" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="I19" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="120">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -1371,17 +1379,17 @@
         <v>40</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H20" s="4"/>
-      <c r="I20" s="31" t="s">
+      <c r="I20" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="J20" s="30" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J20" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1398,12 +1406,12 @@
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="4"/>
-      <c r="I21" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J21" s="28"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I21" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" s="24"/>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -1420,12 +1428,12 @@
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J22" s="28"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I22" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" s="24"/>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -1442,12 +1450,12 @@
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J23" s="28"/>
-    </row>
-    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="I23" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J23" s="24"/>
+    </row>
+    <row r="24" spans="1:10" ht="30">
       <c r="A24" s="5" t="s">
         <v>30</v>
       </c>
@@ -1468,14 +1476,14 @@
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="31" t="s">
+      <c r="I24" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="J24" s="30" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="J24" s="26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="30">
       <c r="A25" s="6" t="s">
         <v>31</v>
       </c>
@@ -1492,12 +1500,12 @@
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="4"/>
-      <c r="I25" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J25" s="28"/>
-    </row>
-    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="I25" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J25" s="24"/>
+    </row>
+    <row r="26" spans="1:10" ht="30">
       <c r="A26" s="6" t="s">
         <v>32</v>
       </c>
@@ -1518,12 +1526,12 @@
       </c>
       <c r="G26" s="17"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J26" s="28"/>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I26" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26" s="24"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" thickBot="1">
       <c r="A27" s="7">
         <v>22</v>
       </c>
@@ -1540,10 +1548,10 @@
       </c>
       <c r="G27" s="23"/>
       <c r="H27" s="8"/>
-      <c r="I27" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J27" s="28"/>
+      <c r="I27" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1560,24 +1568,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New tests for windows 0.9.0 release
</commit_message>
<xml_diff>
--- a/QualiMasterApplication/documentation/Testing Protocol.xlsx
+++ b/QualiMasterApplication/documentation/Testing Protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="52">
   <si>
     <t>Result</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>ConfModel needs to be updated. Results based on QM model.</t>
+  </si>
+  <si>
+    <t>Only Algorithm tested</t>
+  </si>
+  <si>
+    <t>DM constraints are added and removed. For pipeline constraints: constraints are added and shown in the property view. But upon pressin … to access them an empty window opens (so nothing to edit). After restarting model is broken.</t>
+  </si>
+  <si>
+    <t>Roman: 0.9.0 win 64-bit (2016-03-17), Windows 7 64-bit, Java jdk1.8.0_74 64-bit with QM model</t>
   </si>
 </sst>
 </file>
@@ -298,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -365,6 +374,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -380,10 +398,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -688,7 +706,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -700,7 +718,7 @@
     <col min="5" max="5" width="15" style="11" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="11"/>
     <col min="7" max="7" width="58.28515625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="11"/>
+    <col min="8" max="8" width="18.140625" style="11" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" style="11" customWidth="1"/>
     <col min="10" max="10" width="52.140625" style="11" customWidth="1"/>
     <col min="11" max="11" width="23" style="11" customWidth="1"/>
@@ -710,17 +728,19 @@
     <row r="1" spans="1:11">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="4" t="s">
@@ -738,9 +758,15 @@
       <c r="E2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="18"/>
+      <c r="F2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="18"/>
@@ -756,6 +782,9 @@
         <v>40</v>
       </c>
       <c r="E3" s="12"/>
+      <c r="F3" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H3" s="20"/>
       <c r="K3" s="20"/>
     </row>
@@ -770,6 +799,9 @@
         <v>40</v>
       </c>
       <c r="E4" s="10"/>
+      <c r="F4" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H4" s="20"/>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
@@ -785,6 +817,9 @@
         <v>40</v>
       </c>
       <c r="E5" s="10"/>
+      <c r="F5" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
@@ -800,6 +835,9 @@
         <v>40</v>
       </c>
       <c r="E6" s="10"/>
+      <c r="F6" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H6" s="20"/>
       <c r="K6" s="21"/>
     </row>
@@ -814,6 +852,9 @@
         <v>40</v>
       </c>
       <c r="E7" s="10"/>
+      <c r="F7" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H7" s="20"/>
       <c r="K7" s="20"/>
     </row>
@@ -828,9 +869,12 @@
         <v>40</v>
       </c>
       <c r="E8" s="12"/>
+      <c r="F8" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H8" s="20"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
       <c r="K8" s="20"/>
     </row>
     <row r="9" spans="1:11">
@@ -840,16 +884,19 @@
       <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="25" t="s">
         <v>41</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="10"/>
+      <c r="F9" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H9" s="20"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
       <c r="K9" s="20"/>
     </row>
     <row r="10" spans="1:11">
@@ -863,6 +910,9 @@
         <v>40</v>
       </c>
       <c r="E10" s="10"/>
+      <c r="F10" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H10" s="20"/>
       <c r="K10" s="20"/>
     </row>
@@ -877,6 +927,9 @@
         <v>40</v>
       </c>
       <c r="E11" s="10"/>
+      <c r="F11" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H11" s="20"/>
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
@@ -888,13 +941,19 @@
       <c r="B12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="26" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="10"/>
+      <c r="F12" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>43</v>
+      </c>
       <c r="H12" s="20"/>
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
@@ -906,7 +965,7 @@
       <c r="B13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="26" t="s">
         <v>40</v>
       </c>
       <c r="D13" s="11" t="s">
@@ -914,6 +973,12 @@
       </c>
       <c r="E13" s="10" t="s">
         <v>44</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="H13" s="20"/>
       <c r="J13" s="20"/>
@@ -930,6 +995,9 @@
         <v>40</v>
       </c>
       <c r="E14" s="10"/>
+      <c r="F14" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H14" s="20"/>
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
@@ -941,13 +1009,16 @@
       <c r="B15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="26" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>46</v>
       </c>
       <c r="E15" s="10"/>
+      <c r="F15" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H15" s="20"/>
       <c r="K15" s="20"/>
     </row>
@@ -962,6 +1033,9 @@
         <v>40</v>
       </c>
       <c r="E16" s="10"/>
+      <c r="F16" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H16" s="20"/>
       <c r="J16" s="20"/>
       <c r="K16" s="20"/>
@@ -977,6 +1051,9 @@
         <v>40</v>
       </c>
       <c r="E17" s="10"/>
+      <c r="F17" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H17" s="20"/>
       <c r="J17" s="20"/>
       <c r="K17" s="20"/>
@@ -992,6 +1069,9 @@
         <v>40</v>
       </c>
       <c r="E18" s="10"/>
+      <c r="F18" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H18" s="20"/>
       <c r="J18" s="20"/>
       <c r="K18" s="20"/>
@@ -1007,6 +1087,9 @@
         <v>40</v>
       </c>
       <c r="E19" s="10"/>
+      <c r="F19" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H19" s="20"/>
       <c r="J19" s="20"/>
       <c r="K19" s="20"/>
@@ -1025,20 +1108,26 @@
       <c r="H20" s="20"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" ht="60">
       <c r="A21" s="9">
         <v>19</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="25" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>47</v>
       </c>
       <c r="E21" s="10"/>
+      <c r="F21" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="H21" s="20"/>
       <c r="K21" s="20"/>
     </row>
@@ -1053,6 +1142,9 @@
         <v>40</v>
       </c>
       <c r="E22" s="10"/>
+      <c r="F22" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H22" s="20"/>
       <c r="J22" s="20"/>
       <c r="K22" s="20"/>
@@ -1068,6 +1160,9 @@
         <v>40</v>
       </c>
       <c r="E23" s="10"/>
+      <c r="F23" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H23" s="20"/>
       <c r="J23" s="20"/>
       <c r="K23" s="20"/>
@@ -1079,10 +1174,13 @@
       <c r="B24" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="25" t="s">
         <v>41</v>
       </c>
       <c r="E24" s="10"/>
+      <c r="F24" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H24" s="20"/>
       <c r="J24" s="20"/>
       <c r="K24" s="20"/>
@@ -1098,6 +1196,9 @@
         <v>40</v>
       </c>
       <c r="E25" s="10"/>
+      <c r="F25" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="H25" s="20"/>
       <c r="J25" s="20"/>
       <c r="K25" s="20"/>
@@ -1109,7 +1210,7 @@
       <c r="B26" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="30" t="s">
+      <c r="C26" s="26" t="s">
         <v>40</v>
       </c>
       <c r="D26" s="11" t="s">
@@ -1126,7 +1227,7 @@
       <c r="B27" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="26" t="s">
         <v>40</v>
       </c>
       <c r="D27" s="11" t="s">
@@ -1144,7 +1245,7 @@
       <c r="B28" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="26" t="s">
         <v>40</v>
       </c>
       <c r="D28" s="11" t="s">
@@ -1162,7 +1263,7 @@
       <c r="B29" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="26" t="s">
         <v>40</v>
       </c>
       <c r="D29" s="11" t="s">
@@ -1180,7 +1281,7 @@
       <c r="B30" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="26" t="s">
         <v>40</v>
       </c>
       <c r="D30" s="11" t="s">

</xml_diff>

<commit_message>
Set Version number to 0.9.0 (ongoing release), test protocol for Linux
</commit_message>
<xml_diff>
--- a/QualiMasterApplication/documentation/Testing Protocol.xlsx
+++ b/QualiMasterApplication/documentation/Testing Protocol.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13290" windowHeight="9285"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13290" windowHeight="9285" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="0.8.5" sheetId="4" r:id="rId1"/>
+    <sheet name="0.9.0" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="116">
   <si>
     <t>Result</t>
   </si>
@@ -172,13 +171,225 @@
   </si>
   <si>
     <t>Roman: 0.9.0 win 64-bit (2016-03-17), Windows 7 64-bit, Java jdk1.8.0_74 64-bit with QM model</t>
+  </si>
+  <si>
+    <t>Roman: 0.8.5 win 64-bit (2016-01-11), Windows 7 64-bit, Java jdk1.8.0_66 64-bit</t>
+  </si>
+  <si>
+    <t>Roman: 0.8.5 win 64-bit (2016-01-12), Windows 7 64-bit, Java jdk1.8.0_66 64-bit</t>
+  </si>
+  <si>
+    <t>Sascha: 0.8.5 Linux 64-bit (2016-01-12), Ubuntu 14.04.1 64-bit, Java 1.7.0_65 64-bit</t>
+  </si>
+  <si>
+    <t>new repository configuration window</t>
+  </si>
+  <si>
+    <t>-&gt; test scenarios</t>
+  </si>
+  <si>
+    <t>new message; yes - local data saved, no - data from the repository restored</t>
+  </si>
+  <si>
+    <t>changed</t>
+  </si>
+  <si>
+    <t>pass/?</t>
+  </si>
+  <si>
+    <t>After testing "yes", I'm not able to test "no" as it is only asking the first time. But changes can be reverted using the revert all button.</t>
+  </si>
+  <si>
+    <t>check whether test can be done after switchting from local mode to repository and back</t>
+  </si>
+  <si>
+    <t>Ctrl + Shift + S works also for saving all, but it does not ask. However, this is not part of the testing protocol.</t>
+  </si>
+  <si>
+    <t>no action</t>
+  </si>
+  <si>
+    <t>Cancel instead of Close; when artifact selected in the file tree UI selection jumps to the nesting folder, might be confusing</t>
+  </si>
+  <si>
+    <t>First time when I clicked on browse the artifact tree did not opened (tested on Random Sink), afterwards it opened every time.
+OK works
+Cancel/Close button is missing, I need to click on X.
+Refresh brings me to the root of the tree and closes all member. Thus, I'm lost and I do not know how to navigate back to the qualimaster artifacts.</t>
+  </si>
+  <si>
+    <t>artifact can be selected but is not saved (editor is not set dirty)</t>
+  </si>
+  <si>
+    <t>file issue</t>
+  </si>
+  <si>
+    <t>Selection is possible, but the editor is set dirty after clicking on pipeline editor fieldthen it is possible to save.</t>
+  </si>
+  <si>
+    <t>issue #44</t>
+  </si>
+  <si>
+    <t>error in test specification</t>
+  </si>
+  <si>
+    <t>Revert|all does not exist in scenario 2 (local mode)</t>
+  </si>
+  <si>
+    <t>adjust test spec</t>
+  </si>
+  <si>
+    <t>if machine name is set to "roman" then displayed as "ports" in the view; attribute fileds in the UI of a new added Data Management and Algorithms are smaller</t>
+  </si>
+  <si>
+    <t>file issue, see also issue #34</t>
+  </si>
+  <si>
+    <t>For GP Machines name in the view changes only after restarting app; attribute fileds in the UI of a new added Data Management and Algorithms are smaller;</t>
+  </si>
+  <si>
+    <t>issue #42</t>
+  </si>
+  <si>
+    <t>Deleted element, and directly re-added a new element. This new element is shown inside the TreeView as "ports" independently of ist real name. The name will be displayed corectly after a restart of the tool.</t>
+  </si>
+  <si>
+    <t>for algorithms not clear what to copy from data managemet elements (input of output); nothing can be copied from algorithms;</t>
+  </si>
+  <si>
+    <t>ok for now</t>
+  </si>
+  <si>
+    <t>From sink only output, from source input; when copying it does not add but replaces all fields you already have;</t>
+  </si>
+  <si>
+    <t>deferred</t>
+  </si>
+  <si>
+    <t>Unclear what "connect Family Element to remaining pipeline" means. Which part of the pipeline?</t>
+  </si>
+  <si>
+    <t>clarify test spec</t>
+  </si>
+  <si>
+    <t>pass/fail</t>
+  </si>
+  <si>
+    <t>only for data management and pipeline elements; in pipelines only add and remove constraints, can not save, constraint not checked;</t>
+  </si>
+  <si>
+    <t>Algorithm Family do not have constraints in UI (changed document); in Pipeline Editor possible to add constraint for all elements(after adding click on the diagram space to set editor dirty); in Pipeline editorconstraints not check for syntax (name &gt; 1 can be added)</t>
+  </si>
+  <si>
+    <t>issue #43</t>
+  </si>
+  <si>
+    <t>Pipeline editor does not work, if I click into the properties editor, the cell will only be black
+I do not find the configurable constraints inside the other editors.
+Needed help from Roman to find Constraint editor in ohter editors (only available for sources).
+Added constraint "name.size() &gt; 100" to RandomSource, saved, and pressed validate -&gt; No error detected.</t>
+  </si>
+  <si>
+    <t>21--1</t>
+  </si>
+  <si>
+    <t>No manager is assigned in Machines</t>
+  </si>
+  <si>
+    <t>nimbus1.sse.local is also a manager so only 1 error found</t>
+  </si>
+  <si>
+    <t>role is not decorated, everything else is decorated correctly</t>
+  </si>
+  <si>
+    <t>issue #45</t>
+  </si>
+  <si>
+    <t>21--2</t>
+  </si>
+  <si>
+    <t>21--3</t>
+  </si>
+  <si>
+    <t>Input/output mismatch between Family Elements</t>
+  </si>
+  <si>
+    <t>in the editor elements stay maked red after error is fixed and validation was ok</t>
+  </si>
+  <si>
+    <t>see also issue #38</t>
+  </si>
+  <si>
+    <t>Sascha: 0.9.0 Linux 64-bit (2016-03-18), Ubuntu 14.04 64-bit,OpenJDK 64-Bit 1.7.0_65 with ConfModel</t>
+  </si>
+  <si>
+    <t>Choosing yes in Dialog: Model will not be overwritten, but next time, the dialog will not appear. Thus, resetting is only possible via the menu after the tool was started
+No: Works as specified</t>
+  </si>
+  <si>
+    <t>Saving with Crtl + Shift + S saves all without confirmation dialog as it appears with model -&gt; save all.
+Ctrl + S works</t>
+  </si>
+  <si>
+    <t>Adding a new machine, renaming the machine after creation (and saving), will not rearange the machine to the correct domain. This will be done after restarting the app.</t>
+  </si>
+  <si>
+    <t>Contrary to specification: Revert needs a logged in user (oly scenario 1, not 2). Unclear what is ment by demo mode for testing the release version.</t>
+  </si>
+  <si>
+    <t>dynamic-graph-compilation:0.1-SNAPSHOT: Complains that no (campatible manifest was found). Parameters are not taken over.</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>Unlees the part with "re-oppening the editor", this is like scenario 3.</t>
+  </si>
+  <si>
+    <t>New machines, which are not configured, will be added to the domain: "*.softnet.tuc.gr". Desired?</t>
+  </si>
+  <si>
+    <t>Active pipeleines cannot be deleted as they are referenced "by other parts of the model"</t>
+  </si>
+  <si>
+    <t>No ContentAssist, but I also do not have one in Eclipse (when running the Ubuntu VM).</t>
+  </si>
+  <si>
+    <t>Also not for Runtime</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>When clicking on the PDFs, it shows me a message "Missing Plug-in".</t>
+  </si>
+  <si>
+    <t>After multiple failures in a row, the red icon did not disappered in the treeview when fixing the model.
+Cf. Screenshot</t>
+  </si>
+  <si>
+    <t>Names in error message are different than specified in test documentation:
+Description Resource Path Location Type
+Input and output types should be the same Please check: "f5" in PipelineVar_8Cfg, "input item types" in Pipelines//attributeAssignment, "flow end" in Pipelines, "outgoing flows" in Pipelines, "CorrelationComputation" in PipelineVar_8Cfg or "preprocessor" in PipelineVar_8Cfg   Unknown Problem
+Input and output types should be the same Please check: "f8" in PipelineVar_7Cfg, "input item types" in Pipelines//attributeAssignment, "outgoing flows" in Pipelines, "flow end" in Pipelines, "correlation" in PipelineVar_7Cfg or "preprocessor" in PipelineVar_7Cfg   Unknown Problem
+Input and output types should be the same Please check: "fl2" in PipelineVar_6Cfg, "input item types" in Pipelines//attributeAssignment, "flow end" in Pipelines, "outgoing flows" in Pipelines, "MutualInform" in PipelineVar_6Cfg or "Preproc" in PipelineVar_6Cfg   Unknown Problem
+Input and output types should be the same Please check: "Preprocessor" in PriorityPipCfg, "input item types" in Pipelines//attributeAssignment, "flow end" in Pipelines, "outgoing flows" in Pipelines, "f2" in PriorityPipCfg or "FinancialCorrelation" in PriorityPipCfg   Unknown Problem
+Output of at least one algorithm in the Family does not match the output of the Family Please check: "fPreprocessor" in Algorithm Families, "output fields" in Algorithm Families, "Preprocessor" in Algorithms, "output fields" in Algorithms or "members" in Algorithm Families   Unknown Problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It shows me 3 errors (instead of 2). F2 is also marked red:
+Description Resource Path Location Type
+Input and output types should be the same Please check: "outgoing flows" in Pipelines, "f1" in PriorityPipCfg, "flow end" in Pipelines, "mismatch" in PriorityPipCfg, "Preprocessor" in PriorityPipCfg, "FinancialDataSource" in PriorityPipCfg, "m1" in PriorityPipCfg, "f3" in PriorityPipCfg or "input item types" in Pipelines//attributeAssignment   Unknown Problem
+Input and output types should be the same Please check: "outgoing flows" in Pipelines, "f2" in PriorityPipCfg, "flow end" in Pipelines, "Preprocessor" in PriorityPipCfg or "input item types" in Pipelines//attributeAssignment   Unknown Problem
+Input and output types should be the same Please check: "outgoing flows" in Pipelines, "m2" in PriorityPipCfg, "flow end" in Pipelines, "mismatch" in PriorityPipCfg, "Preprocessor" in PriorityPipCfg or "input item types" in Pipelines//attributeAssignment   Unknown Problem
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,7 +406,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,8 +425,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -303,11 +532,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -360,16 +598,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -383,6 +615,117 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -392,21 +735,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -418,10 +752,151 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>6972</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>409574</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>552450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21076272" y="2505075"/>
+          <a:ext cx="3450602" cy="4229100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>53256</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>409576</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21122556" y="7362825"/>
+          <a:ext cx="7061920" cy="4400550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>552450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1662113</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="22164675" y="5695950"/>
+          <a:ext cx="8083550" cy="6062663"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -459,7 +934,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -493,6 +968,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -527,9 +1003,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -702,16 +1179,766 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K27"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" style="54" customWidth="1"/>
+    <col min="2" max="2" width="49.140625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="30"/>
+    <col min="4" max="4" width="65" style="30" customWidth="1"/>
+    <col min="5" max="5" width="15" style="30" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="30"/>
+    <col min="7" max="7" width="58.28515625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="30"/>
+    <col min="9" max="9" width="14.28515625" style="30" customWidth="1"/>
+    <col min="10" max="10" width="52.140625" style="30" customWidth="1"/>
+    <col min="11" max="11" width="23" style="30" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="57"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="57"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="38">
+        <v>1</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="41"/>
+      <c r="H3"/>
+      <c r="I3" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="38">
+        <v>2</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="41"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="41"/>
+      <c r="H4"/>
+      <c r="I4" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4"/>
+      <c r="K4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="38">
+        <v>3</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="41"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="41"/>
+      <c r="H5"/>
+      <c r="I5" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5"/>
+      <c r="K5"/>
+    </row>
+    <row r="6" spans="1:11" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="38">
+        <v>4</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="41"/>
+      <c r="H6"/>
+      <c r="I6" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6" s="44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="38">
+        <v>5</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="41"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="41"/>
+      <c r="H7"/>
+      <c r="I7" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="38">
+        <v>6</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="41"/>
+      <c r="H8"/>
+      <c r="I8" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8"/>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="38">
+        <v>7</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="61"/>
+      <c r="K9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="38">
+        <v>8</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="41"/>
+      <c r="H10"/>
+      <c r="I10" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="K10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="38">
+        <v>9</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="41"/>
+      <c r="H11"/>
+      <c r="I11" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11"/>
+      <c r="K11"/>
+    </row>
+    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="38">
+        <v>10</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12"/>
+      <c r="K12"/>
+    </row>
+    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="38">
+        <v>11</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="41"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="41"/>
+      <c r="H13"/>
+      <c r="I13" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13"/>
+      <c r="K13"/>
+    </row>
+    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="38">
+        <v>12</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="41"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="41"/>
+      <c r="H14"/>
+      <c r="I14" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="K14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="38">
+        <v>13</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="41"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="41"/>
+      <c r="H15"/>
+      <c r="I15" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15"/>
+      <c r="K15"/>
+    </row>
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="38">
+        <v>14</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16"/>
+      <c r="K16"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="38">
+        <v>15</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="41"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="41"/>
+      <c r="H17"/>
+      <c r="I17" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17"/>
+      <c r="K17"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="38">
+        <v>16</v>
+      </c>
+      <c r="B18" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="41"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="41"/>
+      <c r="H18"/>
+      <c r="I18" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J18"/>
+      <c r="K18"/>
+    </row>
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="38">
+        <v>17</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="41"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="41"/>
+      <c r="H19"/>
+      <c r="I19" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="K19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A20" s="38">
+        <v>18</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="39"/>
+      <c r="F20" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="H20" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="K20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="38">
+        <v>19</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="41"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="41"/>
+      <c r="H21"/>
+      <c r="I21" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J21"/>
+      <c r="K21"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="38">
+        <v>20</v>
+      </c>
+      <c r="B22" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="41"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="41"/>
+      <c r="H22"/>
+      <c r="I22" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22"/>
+      <c r="K22"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="38">
+        <v>21</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="41"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="41"/>
+      <c r="H23"/>
+      <c r="I23" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23"/>
+      <c r="K23"/>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="41"/>
+      <c r="H24"/>
+      <c r="I24" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="J24" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="K24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="41"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="41"/>
+      <c r="H25"/>
+      <c r="I25" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J25"/>
+      <c r="K25"/>
+    </row>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="F26" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="41"/>
+      <c r="H26"/>
+      <c r="I26" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J26"/>
+      <c r="K26"/>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="50">
+        <v>22</v>
+      </c>
+      <c r="B27" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="53"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="53"/>
+      <c r="H27"/>
+      <c r="I27" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J27"/>
+      <c r="K27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="I23" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="19" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="18" customWidth="1"/>
     <col min="2" max="2" width="49.140625" style="11" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="11"/>
     <col min="4" max="4" width="65" style="11" customWidth="1"/>
@@ -720,29 +1947,31 @@
     <col min="7" max="7" width="58.28515625" style="11" customWidth="1"/>
     <col min="8" max="8" width="18.140625" style="11" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" style="11" customWidth="1"/>
-    <col min="10" max="10" width="52.140625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="105" style="11" customWidth="1"/>
     <col min="11" max="11" width="23" style="11" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="27" t="s">
+      <c r="D1" s="63"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="G1" s="63"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="63"/>
+      <c r="K1" s="64"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -761,17 +1990,23 @@
       <c r="F2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="18"/>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="I2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -785,10 +2020,13 @@
       <c r="F3" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="K3" s="20"/>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="H3" s="19"/>
+      <c r="I3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="12"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -802,11 +2040,13 @@
       <c r="F4" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="H4" s="19"/>
+      <c r="I4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -820,11 +2060,13 @@
       <c r="F5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-    </row>
-    <row r="6" spans="1:11" ht="32.25" customHeight="1">
+      <c r="H5" s="19"/>
+      <c r="I5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -838,10 +2080,16 @@
       <c r="F6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="K6" s="21"/>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="H6" s="19"/>
+      <c r="I6" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -855,10 +2103,16 @@
       <c r="F7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="20"/>
-      <c r="K7" s="20"/>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="H7" s="19"/>
+      <c r="I7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -872,19 +2126,20 @@
       <c r="F8" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="20"/>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="H8" s="19"/>
+      <c r="I8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="12"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>7</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="23" t="s">
         <v>41</v>
       </c>
       <c r="D9" s="11" t="s">
@@ -894,12 +2149,13 @@
       <c r="F9" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="20"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="20"/>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="H9" s="19"/>
+      <c r="I9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -913,10 +2169,16 @@
       <c r="F10" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="20"/>
-      <c r="K10" s="20"/>
-    </row>
-    <row r="11" spans="1:11" ht="45">
+      <c r="H10" s="19"/>
+      <c r="I10" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -930,42 +2192,49 @@
       <c r="F11" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-    </row>
-    <row r="12" spans="1:11" ht="45">
+      <c r="H11" s="19"/>
+      <c r="I11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="24" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="10"/>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="25" t="s">
         <v>40</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-    </row>
-    <row r="13" spans="1:11" ht="30">
+      <c r="H12" s="19"/>
+      <c r="I12" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>11</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="24" t="s">
         <v>40</v>
       </c>
       <c r="D13" s="11" t="s">
@@ -980,11 +2249,16 @@
       <c r="G13" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-    </row>
-    <row r="14" spans="1:11" ht="45">
+      <c r="H13" s="19"/>
+      <c r="I13" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="K13" s="10"/>
+    </row>
+    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
@@ -998,18 +2272,23 @@
       <c r="F14" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-    </row>
-    <row r="15" spans="1:11" ht="45">
+      <c r="H14" s="19"/>
+      <c r="I14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="K14" s="10"/>
+    </row>
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>13</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="24" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="11" t="s">
@@ -1019,10 +2298,16 @@
       <c r="F15" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="20"/>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16" spans="1:11" ht="45">
+      <c r="H15" s="19"/>
+      <c r="I15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="K15" s="10"/>
+    </row>
+    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>14</v>
       </c>
@@ -1036,11 +2321,13 @@
       <c r="F16" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="H16" s="19"/>
+      <c r="I16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K16" s="10"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>15</v>
       </c>
@@ -1054,11 +2341,13 @@
       <c r="F17" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="H17" s="19"/>
+      <c r="I17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K17" s="10"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>16</v>
       </c>
@@ -1072,11 +2361,13 @@
       <c r="F18" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="H18" s="19"/>
+      <c r="I18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K18" s="10"/>
+    </row>
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>17</v>
       </c>
@@ -1090,11 +2381,16 @@
       <c r="F19" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="H19" s="19"/>
+      <c r="I19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="K19" s="10"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>18</v>
       </c>
@@ -1105,33 +2401,42 @@
         <v>40</v>
       </c>
       <c r="E20" s="10"/>
-      <c r="H20" s="20"/>
-      <c r="K20" s="20"/>
-    </row>
-    <row r="21" spans="1:11" ht="60">
+      <c r="H20" s="19"/>
+      <c r="I20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K20" s="10"/>
+    </row>
+    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>19</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="23" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>47</v>
       </c>
       <c r="E21" s="10"/>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="26" t="s">
         <v>41</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="H21" s="20"/>
-      <c r="K21" s="20"/>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="H21" s="19"/>
+      <c r="I21" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="K21" s="10"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>20</v>
       </c>
@@ -1145,11 +2450,13 @@
       <c r="F22" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="H22" s="19"/>
+      <c r="I22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K22" s="10"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>21</v>
       </c>
@@ -1163,29 +2470,39 @@
       <c r="F23" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="H23" s="19"/>
+      <c r="I23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="K23" s="10"/>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>22</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="23" t="s">
         <v>41</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="H24" s="19"/>
+      <c r="I24" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="K24" s="10"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>23</v>
       </c>
@@ -1199,148 +2516,154 @@
       <c r="F25" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="H25" s="19"/>
+      <c r="I25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K25" s="10"/>
+    </row>
+    <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="24" t="s">
         <v>40</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E26" s="12"/>
-      <c r="H26" s="20"/>
-      <c r="K26" s="20"/>
-    </row>
-    <row r="27" spans="1:11" ht="30">
+      <c r="H26" s="19"/>
+      <c r="I26" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="K26" s="12"/>
+    </row>
+    <row r="27" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="24" t="s">
         <v>40</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E27" s="10"/>
-      <c r="H27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="H27" s="19"/>
+      <c r="I27" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="K27" s="10"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>34</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="24" t="s">
         <v>40</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E28" s="10"/>
-      <c r="H28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-    </row>
-    <row r="29" spans="1:11" ht="30">
+      <c r="H28" s="19"/>
+      <c r="I28" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K28" s="10"/>
+    </row>
+    <row r="29" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="24" t="s">
         <v>40</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E29" s="10"/>
-      <c r="H29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-    </row>
-    <row r="30" spans="1:11" ht="30">
+      <c r="H29" s="19"/>
+      <c r="I29" s="65" t="s">
+        <v>111</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="K29" s="10"/>
+    </row>
+    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="24" t="s">
         <v>40</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E30" s="10"/>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="I30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K30" s="10"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>24</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="20" t="s">
         <v>23</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A32" s="23"/>
+      <c r="I31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K31" s="10"/>
+    </row>
+    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="21"/>
       <c r="B32" s="15"/>
       <c r="C32" s="16"/>
       <c r="D32" s="17"/>
       <c r="E32" s="15"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="3">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
On goning release (0.9.0): New tests on Linux
</commit_message>
<xml_diff>
--- a/QualiMasterApplication/documentation/Testing Protocol.xlsx
+++ b/QualiMasterApplication/documentation/Testing Protocol.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="119">
   <si>
     <t>Result</t>
   </si>
@@ -383,6 +383,15 @@
 Input and output types should be the same Please check: "outgoing flows" in Pipelines, "f2" in PriorityPipCfg, "flow end" in Pipelines, "Preprocessor" in PriorityPipCfg or "input item types" in Pipelines//attributeAssignment   Unknown Problem
 Input and output types should be the same Please check: "outgoing flows" in Pipelines, "m2" in PriorityPipCfg, "flow end" in Pipelines, "mismatch" in PriorityPipCfg, "Preprocessor" in PriorityPipCfg or "input item types" in Pipelines//attributeAssignment   Unknown Problem
 </t>
+  </si>
+  <si>
+    <t>Sascha: 0.9.0 Linux 64-bit (2016-03-21), revalidation of major issues</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
+  <si>
+    <t>spec. Fixed</t>
   </si>
 </sst>
 </file>
@@ -545,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -708,6 +717,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -735,8 +747,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -837,16 +852,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>552450</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>1662113</xdr:rowOff>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>661988</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -870,7 +885,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="22164675" y="5695950"/>
+          <a:off x="27041475" y="1838325"/>
           <a:ext cx="8083550" cy="6062663"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1205,21 +1220,21 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="57"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="56" t="s">
+      <c r="D1" s="58"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="57"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="59" t="s">
+      <c r="G1" s="58"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -1410,10 +1425,10 @@
       </c>
       <c r="G8" s="41"/>
       <c r="H8"/>
-      <c r="I8" s="60" t="s">
+      <c r="I8" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="61" t="s">
+      <c r="J8" s="62" t="s">
         <v>65</v>
       </c>
       <c r="K8"/>
@@ -1441,8 +1456,8 @@
         <v>68</v>
       </c>
       <c r="H9"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="62"/>
       <c r="K9" t="s">
         <v>69</v>
       </c>
@@ -1927,13 +1942,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="I23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="K22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L29" sqref="L29"/>
+      <selection pane="bottomRight" activeCell="L1" sqref="L1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1949,29 +1964,37 @@
     <col min="9" max="9" width="14.28515625" style="11" customWidth="1"/>
     <col min="10" max="10" width="105" style="11" customWidth="1"/>
     <col min="11" max="11" width="23" style="11" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="11"/>
+    <col min="12" max="12" width="27.42578125" style="11" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="62" t="s">
+      <c r="D1" s="64"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="63"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="62" t="s">
+      <c r="G1" s="64"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="63" t="s">
         <v>99</v>
       </c>
-      <c r="J1" s="63"/>
-      <c r="K1" s="64"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J1" s="64"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="66" t="s">
+        <v>116</v>
+      </c>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -2006,7 +2029,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -2025,8 +2048,11 @@
         <v>40</v>
       </c>
       <c r="K3" s="12"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -2046,7 +2072,7 @@
       </c>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -2066,7 +2092,7 @@
       </c>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -2089,7 +2115,7 @@
       </c>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -2112,7 +2138,7 @@
       </c>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -2132,7 +2158,7 @@
       </c>
       <c r="K8" s="12"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>7</v>
       </c>
@@ -2155,7 +2181,7 @@
       </c>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -2177,8 +2203,11 @@
         <v>103</v>
       </c>
       <c r="K10" s="10"/>
-    </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="L10" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -2198,7 +2227,7 @@
       </c>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
@@ -2226,8 +2255,11 @@
         <v>102</v>
       </c>
       <c r="K12" s="10"/>
-    </row>
-    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="L12" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>11</v>
       </c>
@@ -2257,8 +2289,11 @@
         <v>104</v>
       </c>
       <c r="K13" s="10"/>
-    </row>
-    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="L13" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
@@ -2281,7 +2316,7 @@
       </c>
       <c r="K14" s="10"/>
     </row>
-    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>13</v>
       </c>
@@ -2307,7 +2342,7 @@
       </c>
       <c r="K15" s="10"/>
     </row>
-    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>14</v>
       </c>
@@ -2327,7 +2362,7 @@
       </c>
       <c r="K16" s="10"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>15</v>
       </c>
@@ -2347,7 +2382,7 @@
       </c>
       <c r="K17" s="10"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>16</v>
       </c>
@@ -2367,7 +2402,7 @@
       </c>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>17</v>
       </c>
@@ -2390,7 +2425,7 @@
       </c>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>18</v>
       </c>
@@ -2407,7 +2442,7 @@
       </c>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>19</v>
       </c>
@@ -2436,7 +2471,7 @@
       </c>
       <c r="K21" s="10"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>20</v>
       </c>
@@ -2456,7 +2491,7 @@
       </c>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>21</v>
       </c>
@@ -2479,7 +2514,7 @@
       </c>
       <c r="K23" s="10"/>
     </row>
-    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>22</v>
       </c>
@@ -2501,8 +2536,11 @@
         <v>112</v>
       </c>
       <c r="K24" s="10"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>23</v>
       </c>
@@ -2522,7 +2560,7 @@
       </c>
       <c r="K25" s="10"/>
     </row>
-    <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>31</v>
       </c>
@@ -2544,8 +2582,11 @@
         <v>113</v>
       </c>
       <c r="K26" s="12"/>
-    </row>
-    <row r="27" spans="1:11" ht="255" x14ac:dyDescent="0.25">
+      <c r="L26" s="23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="255" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>32</v>
       </c>
@@ -2568,7 +2609,7 @@
       </c>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>34</v>
       </c>
@@ -2588,7 +2629,7 @@
       </c>
       <c r="K28" s="10"/>
     </row>
-    <row r="29" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>36</v>
       </c>
@@ -2603,7 +2644,7 @@
       </c>
       <c r="E29" s="10"/>
       <c r="H29" s="19"/>
-      <c r="I29" s="65" t="s">
+      <c r="I29" s="56" t="s">
         <v>111</v>
       </c>
       <c r="J29" s="11" t="s">
@@ -2611,7 +2652,7 @@
       </c>
       <c r="K29" s="10"/>
     </row>
-    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>38</v>
       </c>
@@ -2630,7 +2671,7 @@
       </c>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>24</v>
       </c>
@@ -2646,7 +2687,7 @@
       </c>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="21"/>
       <c r="B32" s="15"/>
       <c r="C32" s="16"/>
@@ -2657,10 +2698,11 @@
       <c r="K32" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
test protocol for current release (0.9.0), test spec. updated
</commit_message>
<xml_diff>
--- a/QualiMasterApplication/documentation/Testing Protocol.xlsx
+++ b/QualiMasterApplication/documentation/Testing Protocol.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="126">
   <si>
     <t>Result</t>
   </si>
@@ -366,15 +366,6 @@
   <si>
     <t>After multiple failures in a row, the red icon did not disappered in the treeview when fixing the model.
 Cf. Screenshot</t>
-  </si>
-  <si>
-    <t>Names in error message are different than specified in test documentation:
-Description Resource Path Location Type
-Input and output types should be the same Please check: "f5" in PipelineVar_8Cfg, "input item types" in Pipelines//attributeAssignment, "flow end" in Pipelines, "outgoing flows" in Pipelines, "CorrelationComputation" in PipelineVar_8Cfg or "preprocessor" in PipelineVar_8Cfg   Unknown Problem
-Input and output types should be the same Please check: "f8" in PipelineVar_7Cfg, "input item types" in Pipelines//attributeAssignment, "outgoing flows" in Pipelines, "flow end" in Pipelines, "correlation" in PipelineVar_7Cfg or "preprocessor" in PipelineVar_7Cfg   Unknown Problem
-Input and output types should be the same Please check: "fl2" in PipelineVar_6Cfg, "input item types" in Pipelines//attributeAssignment, "flow end" in Pipelines, "outgoing flows" in Pipelines, "MutualInform" in PipelineVar_6Cfg or "Preproc" in PipelineVar_6Cfg   Unknown Problem
-Input and output types should be the same Please check: "Preprocessor" in PriorityPipCfg, "input item types" in Pipelines//attributeAssignment, "flow end" in Pipelines, "outgoing flows" in Pipelines, "f2" in PriorityPipCfg or "FinancialCorrelation" in PriorityPipCfg   Unknown Problem
-Output of at least one algorithm in the Family does not match the output of the Family Please check: "fPreprocessor" in Algorithm Families, "output fields" in Algorithm Families, "Preprocessor" in Algorithms, "output fields" in Algorithms or "members" in Algorithm Families   Unknown Problem</t>
   </si>
   <si>
     <t xml:space="preserve">It shows me 3 errors (instead of 2). F2 is also marked red:
@@ -391,7 +382,36 @@
     <t>fixed</t>
   </si>
   <si>
-    <t>spec. Fixed</t>
+    <t>spec. fixed</t>
+  </si>
+  <si>
+    <t>Sascha: 0.9.0 win 64-bit (2016-03-21), Windows 7 64-bit, Java jdk1.8.0_73 64-bit with QM model</t>
+  </si>
+  <si>
+    <t>Works also in offline mode without running this dioalog before in this workspace.</t>
+  </si>
+  <si>
+    <t>Creating first a family and than an algorithm: The family editor has to be re-opened to make the newly created algorithm selectable (before the new algorithm does no appear / missing refresh of the editor).
+The added algorithm will only be indented below the family in the tree editor after a restart.</t>
+  </si>
+  <si>
+    <t>A cloned algorithm will be intented in the same family as the original, but not assigned to the family (cf. 2nd screen shot).
+After saving the family, the cloned algorithm will be removed completly from the tree view</t>
+  </si>
+  <si>
+    <t>Also a quote (") entered in a string field, does not brake the model.
+Over time the backslahes (needed for escaping the quotes) will be copied multiple times</t>
+  </si>
+  <si>
+    <t>QM documentation works, but the tree offers only the documentation to QM. The tree for the EASy-Producer documentation is missing.</t>
+  </si>
+  <si>
+    <t>Adding a new machine may lead to the situation that another machine maybe intentend into the wrong domain temporarily (cf. Screenshot). This will be fixed after resaving this item or after restart.
+Deleting a family containing algorithms lead to an exception and empty family category when opening the algorithms tree. This will also lead to further exceptions when restarting the app and switching from local to online mode. A revert of the model solves this problem.</t>
+  </si>
+  <si>
+    <t>After multiple failures in a row, the red icon did not disappered in the treeview when fixing the model.
+Cf. Screenshot of the Linux test</t>
   </si>
 </sst>
 </file>
@@ -453,7 +473,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -541,20 +561,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -610,128 +621,124 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -747,11 +754,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -852,16 +859,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>942975</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>661988</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -885,8 +892,118 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="27041475" y="1838325"/>
-          <a:ext cx="8083550" cy="6062663"/>
+          <a:off x="26136600" y="2381250"/>
+          <a:ext cx="7315199" cy="5486400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="38757225" y="400050"/>
+          <a:ext cx="2600325" cy="5362575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="38681025" y="5934075"/>
+          <a:ext cx="7153275" cy="1704975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1203,201 +1320,201 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="54" customWidth="1"/>
-    <col min="2" max="2" width="49.140625" style="30" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="30"/>
-    <col min="4" max="4" width="65" style="30" customWidth="1"/>
-    <col min="5" max="5" width="15" style="30" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="30"/>
-    <col min="7" max="7" width="58.28515625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="30"/>
-    <col min="9" max="9" width="14.28515625" style="30" customWidth="1"/>
-    <col min="10" max="10" width="52.140625" style="30" customWidth="1"/>
-    <col min="11" max="11" width="23" style="30" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="30"/>
+    <col min="1" max="1" width="11.7109375" style="52" customWidth="1"/>
+    <col min="2" max="2" width="49.140625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="28"/>
+    <col min="4" max="4" width="65" style="28" customWidth="1"/>
+    <col min="5" max="5" width="15" style="28" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="28"/>
+    <col min="7" max="7" width="58.28515625" style="28" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="28"/>
+    <col min="9" max="9" width="14.28515625" style="28" customWidth="1"/>
+    <col min="10" max="10" width="52.140625" style="28" customWidth="1"/>
+    <col min="11" max="11" width="23" style="28" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="28"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="57" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="57" t="s">
+      <c r="D1" s="56"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="58"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="60" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="37" t="s">
+      <c r="K2" s="35" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="38">
+      <c r="A3" s="36">
         <v>1</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="41" t="s">
+      <c r="C3" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="41"/>
+      <c r="F3" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="39"/>
       <c r="H3"/>
-      <c r="I3" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="30" t="s">
+      <c r="I3" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="28" t="s">
         <v>55</v>
       </c>
       <c r="K3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="38">
+      <c r="A4" s="36">
         <v>2</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="41"/>
+      <c r="C4" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="39"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="39"/>
       <c r="H4"/>
-      <c r="I4" s="30" t="s">
+      <c r="I4" s="28" t="s">
         <v>40</v>
       </c>
       <c r="J4"/>
       <c r="K4"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="38">
+      <c r="A5" s="36">
         <v>3</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="41"/>
+      <c r="C5" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="39"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="39"/>
       <c r="H5"/>
-      <c r="I5" s="30" t="s">
+      <c r="I5" s="28" t="s">
         <v>40</v>
       </c>
       <c r="J5"/>
       <c r="K5"/>
     </row>
     <row r="6" spans="1:11" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38">
+      <c r="A6" s="36">
         <v>4</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="41" t="s">
+      <c r="C6" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="41"/>
+      <c r="F6" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="39"/>
       <c r="H6"/>
-      <c r="I6" s="43" t="s">
+      <c r="I6" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="K6" s="44" t="s">
+      <c r="K6" s="42" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="38">
+      <c r="A7" s="36">
         <v>5</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="41"/>
+      <c r="C7" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="39"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="39"/>
       <c r="H7"/>
-      <c r="I7" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" s="30" t="s">
+      <c r="I7" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="28" t="s">
         <v>62</v>
       </c>
       <c r="K7" t="s">
@@ -1405,84 +1522,84 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="38">
+      <c r="A8" s="36">
         <v>6</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="41" t="s">
+      <c r="C8" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="41"/>
+      <c r="F8" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="39"/>
       <c r="H8"/>
-      <c r="I8" s="61" t="s">
+      <c r="I8" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="62" t="s">
+      <c r="J8" s="60" t="s">
         <v>65</v>
       </c>
       <c r="K8"/>
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="38">
+      <c r="A9" s="36">
         <v>7</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="41" t="s">
+      <c r="F9" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="39" t="s">
         <v>68</v>
       </c>
       <c r="H9"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="62"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="60"/>
       <c r="K9" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="38">
+      <c r="A10" s="36">
         <v>8</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="41"/>
+      <c r="C10" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="39"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="39"/>
       <c r="H10"/>
-      <c r="I10" s="46" t="s">
+      <c r="I10" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="J10" s="30" t="s">
+      <c r="J10" s="28" t="s">
         <v>71</v>
       </c>
       <c r="K10" t="s">
@@ -1490,103 +1607,103 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="38">
+      <c r="A11" s="36">
         <v>9</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="41"/>
+      <c r="C11" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="39"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="39"/>
       <c r="H11"/>
-      <c r="I11" s="30" t="s">
+      <c r="I11" s="28" t="s">
         <v>40</v>
       </c>
       <c r="J11"/>
       <c r="K11"/>
     </row>
     <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="38">
+      <c r="A12" s="36">
         <v>10</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="41" t="s">
+      <c r="C12" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="41" t="s">
+      <c r="F12" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="39" t="s">
         <v>75</v>
       </c>
       <c r="H12" t="s">
         <v>76</v>
       </c>
-      <c r="I12" s="30" t="s">
+      <c r="I12" s="28" t="s">
         <v>40</v>
       </c>
       <c r="J12"/>
       <c r="K12"/>
     </row>
     <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="38">
+      <c r="A13" s="36">
         <v>11</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="41"/>
+      <c r="C13" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="39"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="39"/>
       <c r="H13"/>
-      <c r="I13" s="30" t="s">
+      <c r="I13" s="28" t="s">
         <v>40</v>
       </c>
       <c r="J13"/>
       <c r="K13"/>
     </row>
     <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="38">
+      <c r="A14" s="36">
         <v>12</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="41"/>
+      <c r="C14" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="39"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="39"/>
       <c r="H14"/>
-      <c r="I14" s="47" t="s">
+      <c r="I14" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="J14" s="30" t="s">
+      <c r="J14" s="28" t="s">
         <v>77</v>
       </c>
       <c r="K14" t="s">
@@ -1594,126 +1711,126 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="38">
+      <c r="A15" s="36">
         <v>13</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="41"/>
+      <c r="C15" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="39"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="39"/>
       <c r="H15"/>
-      <c r="I15" s="30" t="s">
+      <c r="I15" s="28" t="s">
         <v>40</v>
       </c>
       <c r="J15"/>
       <c r="K15"/>
     </row>
     <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="38">
+      <c r="A16" s="36">
         <v>14</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="41" t="s">
+      <c r="C16" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="39" t="s">
+      <c r="E16" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="F16" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" s="41" t="s">
+      <c r="F16" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="39" t="s">
         <v>80</v>
       </c>
       <c r="H16" t="s">
         <v>81</v>
       </c>
-      <c r="I16" s="30" t="s">
+      <c r="I16" s="28" t="s">
         <v>40</v>
       </c>
       <c r="J16"/>
       <c r="K16"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="38">
+      <c r="A17" s="36">
         <v>15</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="41"/>
+      <c r="C17" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="39"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="39"/>
       <c r="H17"/>
-      <c r="I17" s="30" t="s">
+      <c r="I17" s="28" t="s">
         <v>40</v>
       </c>
       <c r="J17"/>
       <c r="K17"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="38">
+      <c r="A18" s="36">
         <v>16</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G18" s="41"/>
+      <c r="C18" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="39"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="39"/>
       <c r="H18"/>
-      <c r="I18" s="30" t="s">
+      <c r="I18" s="28" t="s">
         <v>40</v>
       </c>
       <c r="J18"/>
       <c r="K18"/>
     </row>
     <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="38">
+      <c r="A19" s="36">
         <v>17</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="41"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="41"/>
+      <c r="C19" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="39"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="39"/>
       <c r="H19"/>
-      <c r="I19" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="J19" s="30" t="s">
+      <c r="I19" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" s="28" t="s">
         <v>82</v>
       </c>
       <c r="K19" t="s">
@@ -1721,32 +1838,32 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A20" s="38">
+      <c r="A20" s="36">
         <v>18</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="41" t="s">
+      <c r="D20" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="24" t="s">
+      <c r="E20" s="37"/>
+      <c r="F20" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="G20" s="41" t="s">
+      <c r="G20" s="39" t="s">
         <v>86</v>
       </c>
       <c r="H20" t="s">
         <v>87</v>
       </c>
-      <c r="I20" s="47" t="s">
+      <c r="I20" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="30" t="s">
+      <c r="J20" s="28" t="s">
         <v>88</v>
       </c>
       <c r="K20" t="s">
@@ -1754,99 +1871,99 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="38">
+      <c r="A21" s="36">
         <v>19</v>
       </c>
-      <c r="B21" s="39" t="s">
+      <c r="B21" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="41"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G21" s="41"/>
+      <c r="C21" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="39"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="39"/>
       <c r="H21"/>
-      <c r="I21" s="30" t="s">
+      <c r="I21" s="28" t="s">
         <v>40</v>
       </c>
       <c r="J21"/>
       <c r="K21"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="38">
+      <c r="A22" s="36">
         <v>20</v>
       </c>
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="41"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G22" s="41"/>
+      <c r="C22" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="39"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="39"/>
       <c r="H22"/>
-      <c r="I22" s="30" t="s">
+      <c r="I22" s="28" t="s">
         <v>40</v>
       </c>
       <c r="J22"/>
       <c r="K22"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="38">
+      <c r="A23" s="36">
         <v>21</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="41"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G23" s="41"/>
+      <c r="C23" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="39"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="39"/>
       <c r="H23"/>
-      <c r="I23" s="30" t="s">
+      <c r="I23" s="28" t="s">
         <v>40</v>
       </c>
       <c r="J23"/>
       <c r="K23"/>
     </row>
     <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="37" t="s">
         <v>90</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="41" t="s">
+      <c r="D24" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="E24" s="42" t="s">
+      <c r="E24" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="F24" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G24" s="41"/>
+      <c r="F24" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="39"/>
       <c r="H24"/>
-      <c r="I24" s="47" t="s">
+      <c r="I24" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="J24" s="30" t="s">
+      <c r="J24" s="28" t="s">
         <v>92</v>
       </c>
       <c r="K24" t="s">
@@ -1854,73 +1971,73 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="49" t="s">
+      <c r="A25" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="41"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G25" s="41"/>
+      <c r="C25" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="39"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="39"/>
       <c r="H25"/>
-      <c r="I25" s="30" t="s">
+      <c r="I25" s="28" t="s">
         <v>40</v>
       </c>
       <c r="J25"/>
       <c r="K25"/>
     </row>
     <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="41" t="s">
+      <c r="C26" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="E26" s="39" t="s">
+      <c r="E26" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="F26" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G26" s="41"/>
+      <c r="F26" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="39"/>
       <c r="H26"/>
-      <c r="I26" s="30" t="s">
+      <c r="I26" s="28" t="s">
         <v>40</v>
       </c>
       <c r="J26"/>
       <c r="K26"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="50">
+      <c r="A27" s="48">
         <v>22</v>
       </c>
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="53"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="G27" s="53"/>
+      <c r="C27" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="51"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="51"/>
       <c r="H27"/>
-      <c r="I27" s="30" t="s">
+      <c r="I27" s="28" t="s">
         <v>40</v>
       </c>
       <c r="J27"/>
@@ -1942,13 +2059,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="K22" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="N6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L1" sqref="L1:P1"/>
+      <selection pane="bottomRight" activeCell="AI60" sqref="AI60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1964,37 +2081,51 @@
     <col min="9" max="9" width="14.28515625" style="11" customWidth="1"/>
     <col min="10" max="10" width="105" style="11" customWidth="1"/>
     <col min="11" max="11" width="23" style="11" customWidth="1"/>
-    <col min="12" max="12" width="27.42578125" style="11" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="11"/>
+    <col min="12" max="12" width="19.28515625" style="11" customWidth="1"/>
+    <col min="13" max="13" width="45.28515625" style="11" customWidth="1"/>
+    <col min="14" max="20" width="9.140625" style="11"/>
+    <col min="21" max="21" width="9.140625" style="11" customWidth="1"/>
+    <col min="22" max="22" width="62.140625" style="11" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" style="11" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="63" t="s">
+      <c r="D1" s="62"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="64"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="63" t="s">
+      <c r="G1" s="62"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="62" t="s">
         <v>99</v>
       </c>
-      <c r="J1" s="64"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="66" t="s">
-        <v>116</v>
-      </c>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J1" s="62"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="61" t="s">
+        <v>115</v>
+      </c>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="64"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="61" t="s">
+        <v>118</v>
+      </c>
+      <c r="V1" s="62"/>
+      <c r="W1" s="63"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -2010,26 +2141,37 @@
       <c r="E2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="54" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="25" t="s">
         <v>1</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L2" s="1"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -2040,19 +2182,24 @@
         <v>40</v>
       </c>
       <c r="E3" s="12"/>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H3" s="19"/>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="11" t="s">
         <v>40</v>
       </c>
       <c r="K3" s="12"/>
-      <c r="L3" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T3" s="10"/>
+      <c r="U3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W3" s="10"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -2063,16 +2210,22 @@
         <v>40</v>
       </c>
       <c r="E4" s="10"/>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H4" s="19"/>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="11" t="s">
         <v>40</v>
       </c>
       <c r="K4" s="10"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L4" s="1"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W4" s="10"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -2083,16 +2236,22 @@
         <v>40</v>
       </c>
       <c r="E5" s="10"/>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H5" s="19"/>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="11" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="10"/>
-    </row>
-    <row r="6" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="L5" s="1"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W5" s="10"/>
+    </row>
+    <row r="6" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -2103,19 +2262,28 @@
         <v>40</v>
       </c>
       <c r="E6" s="10"/>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H6" s="19"/>
-      <c r="I6" s="55" t="s">
+      <c r="I6" s="23" t="s">
         <v>40</v>
       </c>
       <c r="J6" s="11" t="s">
         <v>100</v>
       </c>
       <c r="K6" s="10"/>
-    </row>
-    <row r="7" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="L6" s="1"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="V6" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="W6" s="10"/>
+    </row>
+    <row r="7" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -2126,19 +2294,25 @@
         <v>40</v>
       </c>
       <c r="E7" s="10"/>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H7" s="19"/>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="11" t="s">
         <v>40</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>101</v>
       </c>
       <c r="K7" s="10"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L7" s="1"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W7" s="10"/>
+    </row>
+    <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -2149,39 +2323,54 @@
         <v>40</v>
       </c>
       <c r="E8" s="12"/>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H8" s="19"/>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="11" t="s">
         <v>40</v>
       </c>
       <c r="K8" s="12"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L8" s="1"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V8" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="W8" s="10"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>7</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="21" t="s">
         <v>41</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="10"/>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H9" s="19"/>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="11" t="s">
         <v>40</v>
       </c>
       <c r="K9" s="10"/>
-    </row>
-    <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="L9" s="1"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W9" s="10"/>
+    </row>
+    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -2192,22 +2381,27 @@
         <v>40</v>
       </c>
       <c r="E10" s="10"/>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H10" s="19"/>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="23" t="s">
         <v>40</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>103</v>
       </c>
       <c r="K10" s="10"/>
-      <c r="L10" s="11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="L10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T10" s="10"/>
+      <c r="U10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W10" s="10"/>
+    </row>
+    <row r="11" spans="1:23" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -2218,55 +2412,72 @@
         <v>40</v>
       </c>
       <c r="E11" s="10"/>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H11" s="19"/>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="11" t="s">
         <v>40</v>
       </c>
       <c r="K11" s="10"/>
-    </row>
-    <row r="12" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="L11" s="1"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="V11" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="W11" s="10"/>
+    </row>
+    <row r="12" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="22" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="10"/>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="22" t="s">
         <v>40</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>43</v>
       </c>
       <c r="H12" s="19"/>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="23" t="s">
         <v>40</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>102</v>
       </c>
       <c r="K12" s="10"/>
-      <c r="L12" s="11" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="L12" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="T12" s="10"/>
+      <c r="U12" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="V12" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="W12" s="10"/>
+    </row>
+    <row r="13" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>11</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="22" t="s">
         <v>40</v>
       </c>
       <c r="D13" s="11" t="s">
@@ -2275,25 +2486,30 @@
       <c r="E13" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>49</v>
       </c>
       <c r="H13" s="19"/>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="24" t="s">
         <v>105</v>
       </c>
       <c r="J13" s="11" t="s">
         <v>104</v>
       </c>
       <c r="K13" s="10"/>
-      <c r="L13" s="11" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="L13" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="T13" s="10"/>
+      <c r="U13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W13" s="10"/>
+    </row>
+    <row r="14" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
@@ -2304,45 +2520,60 @@
         <v>40</v>
       </c>
       <c r="E14" s="10"/>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H14" s="19"/>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="11" t="s">
         <v>40</v>
       </c>
       <c r="J14" s="11" t="s">
         <v>106</v>
       </c>
       <c r="K14" s="10"/>
-    </row>
-    <row r="15" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="L14" s="1"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W14" s="10"/>
+    </row>
+    <row r="15" spans="1:23" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>13</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="22" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>46</v>
       </c>
       <c r="E15" s="10"/>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H15" s="19"/>
-      <c r="I15" s="1" t="s">
+      <c r="I15" s="11" t="s">
         <v>40</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>107</v>
       </c>
       <c r="K15" s="10"/>
-    </row>
-    <row r="16" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="L15" s="1"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="V15" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="W15" s="10"/>
+    </row>
+    <row r="16" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>14</v>
       </c>
@@ -2353,16 +2584,25 @@
         <v>40</v>
       </c>
       <c r="E16" s="10"/>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H16" s="19"/>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="11" t="s">
         <v>40</v>
       </c>
       <c r="K16" s="10"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L16" s="1"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="V16" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="W16" s="10"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>15</v>
       </c>
@@ -2373,16 +2613,22 @@
         <v>40</v>
       </c>
       <c r="E17" s="10"/>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H17" s="19"/>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="11" t="s">
         <v>40</v>
       </c>
       <c r="K17" s="10"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L17" s="1"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W17" s="10"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>16</v>
       </c>
@@ -2393,16 +2639,22 @@
         <v>40</v>
       </c>
       <c r="E18" s="10"/>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H18" s="19"/>
-      <c r="I18" s="1" t="s">
+      <c r="I18" s="11" t="s">
         <v>40</v>
       </c>
       <c r="K18" s="10"/>
-    </row>
-    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L18" s="1"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W18" s="10"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>17</v>
       </c>
@@ -2413,19 +2665,25 @@
         <v>40</v>
       </c>
       <c r="E19" s="10"/>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H19" s="19"/>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="11" t="s">
         <v>40</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>108</v>
       </c>
       <c r="K19" s="10"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L19" s="1"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W19" s="10"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>18</v>
       </c>
@@ -2436,42 +2694,55 @@
         <v>40</v>
       </c>
       <c r="E20" s="10"/>
+      <c r="F20" s="1"/>
       <c r="H20" s="19"/>
-      <c r="I20" s="1" t="s">
+      <c r="I20" s="11" t="s">
         <v>40</v>
       </c>
       <c r="K20" s="10"/>
-    </row>
-    <row r="21" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="L20" s="1"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W20" s="10"/>
+    </row>
+    <row r="21" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>19</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="21" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>47</v>
       </c>
       <c r="E21" s="10"/>
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="21" t="s">
         <v>41</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>50</v>
       </c>
       <c r="H21" s="19"/>
-      <c r="I21" s="24" t="s">
+      <c r="I21" s="23" t="s">
         <v>40</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>109</v>
       </c>
       <c r="K21" s="10"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L21" s="1"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W21" s="10"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>20</v>
       </c>
@@ -2482,16 +2753,22 @@
         <v>40</v>
       </c>
       <c r="E22" s="10"/>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H22" s="19"/>
-      <c r="I22" s="1" t="s">
+      <c r="I22" s="11" t="s">
         <v>40</v>
       </c>
       <c r="K22" s="10"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L22" s="1"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W22" s="10"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>21</v>
       </c>
@@ -2502,45 +2779,62 @@
         <v>40</v>
       </c>
       <c r="E23" s="10"/>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H23" s="19"/>
-      <c r="I23" s="1" t="s">
+      <c r="I23" s="11" t="s">
         <v>40</v>
       </c>
       <c r="J23" s="11" t="s">
         <v>110</v>
       </c>
       <c r="K23" s="10"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L23" s="1"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W23" s="10"/>
+    </row>
+    <row r="24" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>22</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="21" t="s">
         <v>41</v>
       </c>
       <c r="E24" s="10"/>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H24" s="19"/>
-      <c r="I24" s="23" t="s">
+      <c r="I24" s="24" t="s">
         <v>105</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>112</v>
       </c>
       <c r="K24" s="10"/>
-      <c r="L24" s="23" t="s">
+      <c r="L24" s="21" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="T24" s="10"/>
+      <c r="U24" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="V24" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="W24" s="10"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>23</v>
       </c>
@@ -2551,158 +2845,226 @@
         <v>40</v>
       </c>
       <c r="E25" s="10"/>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H25" s="19"/>
-      <c r="I25" s="1" t="s">
+      <c r="I25" s="11" t="s">
         <v>40</v>
       </c>
       <c r="K25" s="10"/>
-    </row>
-    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L25" s="1"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W25" s="10"/>
+    </row>
+    <row r="26" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="22" t="s">
         <v>40</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E26" s="12"/>
+      <c r="F26" s="1"/>
       <c r="H26" s="19"/>
-      <c r="I26" s="23" t="s">
+      <c r="I26" s="24" t="s">
         <v>105</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>113</v>
       </c>
       <c r="K26" s="12"/>
-      <c r="L26" s="23" t="s">
+      <c r="L26" s="21" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="255" x14ac:dyDescent="0.25">
+      <c r="M26" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="T26" s="10"/>
+      <c r="U26" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="V26" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="W26" s="10"/>
+    </row>
+    <row r="27" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="22" t="s">
         <v>40</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E27" s="10"/>
+      <c r="F27" s="1"/>
       <c r="H27" s="19"/>
-      <c r="I27" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="J27" s="11" t="s">
-        <v>114</v>
+      <c r="I27" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="K27" s="10"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L27" s="1"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W27" s="10"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>34</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="22" t="s">
         <v>40</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E28" s="10"/>
+      <c r="F28" s="1"/>
       <c r="H28" s="19"/>
       <c r="I28" s="11" t="s">
         <v>40</v>
       </c>
       <c r="K28" s="10"/>
-    </row>
-    <row r="29" spans="1:12" ht="195" x14ac:dyDescent="0.25">
+      <c r="L28" s="1"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W28" s="10"/>
+    </row>
+    <row r="29" spans="1:23" ht="195" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="22" t="s">
         <v>40</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E29" s="10"/>
+      <c r="F29" s="1"/>
       <c r="H29" s="19"/>
-      <c r="I29" s="56" t="s">
+      <c r="I29" s="65" t="s">
         <v>111</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K29" s="10"/>
-    </row>
-    <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L29" s="1"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W29" s="10"/>
+    </row>
+    <row r="30" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="22" t="s">
         <v>40</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E30" s="10"/>
-      <c r="I30" s="1" t="s">
+      <c r="F30" s="1"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="11" t="s">
         <v>40</v>
       </c>
       <c r="K30" s="10"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L30" s="1"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W30" s="10"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>24</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="19" t="s">
         <v>23</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E31" s="10"/>
-      <c r="I31" s="1" t="s">
+      <c r="F31" s="1"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="11" t="s">
         <v>40</v>
       </c>
       <c r="K31" s="10"/>
-    </row>
-    <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="21"/>
+      <c r="L31" s="1"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W31" s="10"/>
+    </row>
+    <row r="32" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="20"/>
       <c r="B32" s="15"/>
       <c r="C32" s="16"/>
       <c r="D32" s="17"/>
       <c r="E32" s="15"/>
-      <c r="I32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="17"/>
       <c r="J32" s="17"/>
       <c r="K32" s="15"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="15"/>
+      <c r="U32" s="16"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="L1:P1"/>
+    <mergeCell ref="U1:W1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Preparation for a new release. Version changed to 0.9.5, Test scenarios typo fixed, new test protocol for nightly.
</commit_message>
<xml_diff>
--- a/QualiMasterApplication/documentation/Testing Protocol.xlsx
+++ b/QualiMasterApplication/documentation/Testing Protocol.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13290" windowHeight="9285" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13290" windowHeight="9285" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="0.8.5" sheetId="4" r:id="rId1"/>
     <sheet name="0.9.0" sheetId="1" r:id="rId2"/>
+    <sheet name="0.9.5" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="130">
   <si>
     <t>Result</t>
   </si>
@@ -413,12 +414,24 @@
   <si>
     <t>Sascha: 0.9.0 Linux 64-bit (2016-03-18), Ubuntu 14.04 64-bit,OpenJDK 64-Bit 1.7.0_65 with QM model</t>
   </si>
+  <si>
+    <t>new AlgorithFamily is not shown under Algorithms when Algorithm is configured</t>
+  </si>
+  <si>
+    <t>After validating back to Valid machine in the View stays with red cross. Removed after validating next time.</t>
+  </si>
+  <si>
+    <t>no Priority Data Sink anymore</t>
+  </si>
+  <si>
+    <t>Roman: 0.9.5 win 64-bit (2016-04-20), Windows 7 64-bit, Java jdk1.8.0_74 64-bit with QM2 model</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -430,6 +443,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -565,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -760,9 +779,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -878,10 +900,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -901,7 +923,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -933,10 +955,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -956,7 +978,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -988,10 +1010,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1011,7 +1033,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1026,9 +1048,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1066,7 +1088,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1100,7 +1122,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1135,10 +1156,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1311,14 +1331,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="52" customWidth="1"/>
     <col min="2" max="2" width="49.140625" style="28" customWidth="1"/>
@@ -1334,7 +1354,7 @@
     <col min="12" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="26"/>
       <c r="B1" s="27"/>
       <c r="C1" s="57" t="s">
@@ -1353,7 +1373,7 @@
       <c r="J1" s="60"/>
       <c r="K1" s="60"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="29" t="s">
         <v>3</v>
       </c>
@@ -1388,7 +1408,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="30">
       <c r="A3" s="36">
         <v>1</v>
       </c>
@@ -1417,7 +1437,7 @@
       </c>
       <c r="K3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="36">
         <v>2</v>
       </c>
@@ -1440,7 +1460,7 @@
       <c r="J4"/>
       <c r="K4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="36">
         <v>3</v>
       </c>
@@ -1463,7 +1483,7 @@
       <c r="J5"/>
       <c r="K5"/>
     </row>
-    <row r="6" spans="1:11" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="81.75" customHeight="1">
       <c r="A6" s="36">
         <v>4</v>
       </c>
@@ -1494,7 +1514,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="30">
       <c r="A7" s="36">
         <v>5</v>
       </c>
@@ -1521,7 +1541,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="30">
       <c r="A8" s="36">
         <v>6</v>
       </c>
@@ -1550,7 +1570,7 @@
       </c>
       <c r="K8"/>
     </row>
-    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="30">
       <c r="A9" s="36">
         <v>7</v>
       </c>
@@ -1579,7 +1599,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="30">
       <c r="A10" s="36">
         <v>8</v>
       </c>
@@ -1606,7 +1626,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="45">
       <c r="A11" s="36">
         <v>9</v>
       </c>
@@ -1629,7 +1649,7 @@
       <c r="J11"/>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="45">
       <c r="A12" s="36">
         <v>10</v>
       </c>
@@ -1660,7 +1680,7 @@
       <c r="J12"/>
       <c r="K12"/>
     </row>
-    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="45">
       <c r="A13" s="36">
         <v>11</v>
       </c>
@@ -1683,7 +1703,7 @@
       <c r="J13"/>
       <c r="K13"/>
     </row>
-    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="60">
       <c r="A14" s="36">
         <v>12</v>
       </c>
@@ -1710,7 +1730,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="45">
       <c r="A15" s="36">
         <v>13</v>
       </c>
@@ -1733,7 +1753,7 @@
       <c r="J15"/>
       <c r="K15"/>
     </row>
-    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="30">
       <c r="A16" s="36">
         <v>14</v>
       </c>
@@ -1764,7 +1784,7 @@
       <c r="J16"/>
       <c r="K16"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="36">
         <v>15</v>
       </c>
@@ -1787,7 +1807,7 @@
       <c r="J17"/>
       <c r="K17"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="36">
         <v>16</v>
       </c>
@@ -1810,7 +1830,7 @@
       <c r="J18"/>
       <c r="K18"/>
     </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="30">
       <c r="A19" s="36">
         <v>17</v>
       </c>
@@ -1837,7 +1857,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="120">
       <c r="A20" s="36">
         <v>18</v>
       </c>
@@ -1870,7 +1890,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="36">
         <v>19</v>
       </c>
@@ -1893,7 +1913,7 @@
       <c r="J21"/>
       <c r="K21"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="36">
         <v>20</v>
       </c>
@@ -1916,7 +1936,7 @@
       <c r="J22"/>
       <c r="K22"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="36">
         <v>21</v>
       </c>
@@ -1939,7 +1959,7 @@
       <c r="J23"/>
       <c r="K23"/>
     </row>
-    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="30">
       <c r="A24" s="46" t="s">
         <v>89</v>
       </c>
@@ -1970,7 +1990,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="30">
       <c r="A25" s="47" t="s">
         <v>94</v>
       </c>
@@ -1993,7 +2013,7 @@
       <c r="J25"/>
       <c r="K25"/>
     </row>
-    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="30">
       <c r="A26" s="47" t="s">
         <v>95</v>
       </c>
@@ -2020,7 +2040,7 @@
       <c r="J26"/>
       <c r="K26"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="15.75" thickBot="1">
       <c r="A27" s="48">
         <v>22</v>
       </c>
@@ -2058,17 +2078,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="18" customWidth="1"/>
     <col min="2" max="2" width="49.140625" style="11" customWidth="1"/>
@@ -2090,7 +2110,7 @@
     <col min="24" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="63" t="s">
@@ -2125,7 +2145,7 @@
       <c r="V1" s="64"/>
       <c r="W1" s="65"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -2171,7 +2191,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -2199,7 +2219,7 @@
       </c>
       <c r="W3" s="10"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -2225,7 +2245,7 @@
       </c>
       <c r="W4" s="10"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -2251,7 +2271,7 @@
       </c>
       <c r="W5" s="10"/>
     </row>
-    <row r="6" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="60">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -2283,7 +2303,7 @@
       </c>
       <c r="W6" s="10"/>
     </row>
-    <row r="7" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="30">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -2312,7 +2332,7 @@
       </c>
       <c r="W7" s="10"/>
     </row>
-    <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="30">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -2341,7 +2361,7 @@
       </c>
       <c r="W8" s="10"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23">
       <c r="A9" s="9">
         <v>7</v>
       </c>
@@ -2370,7 +2390,7 @@
       </c>
       <c r="W9" s="10"/>
     </row>
-    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="30">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -2401,7 +2421,7 @@
       </c>
       <c r="W10" s="10"/>
     </row>
-    <row r="11" spans="1:23" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="90">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -2430,7 +2450,7 @@
       </c>
       <c r="W11" s="10"/>
     </row>
-    <row r="12" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="45">
       <c r="A12" s="9">
         <v>10</v>
       </c>
@@ -2470,7 +2490,7 @@
       </c>
       <c r="W12" s="10"/>
     </row>
-    <row r="13" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="30">
       <c r="A13" s="9">
         <v>11</v>
       </c>
@@ -2509,7 +2529,7 @@
       </c>
       <c r="W13" s="10"/>
     </row>
-    <row r="14" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="45">
       <c r="A14" s="9">
         <v>12</v>
       </c>
@@ -2538,7 +2558,7 @@
       </c>
       <c r="W14" s="10"/>
     </row>
-    <row r="15" spans="1:23" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="123.75" customHeight="1">
       <c r="A15" s="9">
         <v>13</v>
       </c>
@@ -2573,7 +2593,7 @@
       </c>
       <c r="W15" s="10"/>
     </row>
-    <row r="16" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="60">
       <c r="A16" s="9">
         <v>14</v>
       </c>
@@ -2602,7 +2622,7 @@
       </c>
       <c r="W16" s="10"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23">
       <c r="A17" s="9">
         <v>15</v>
       </c>
@@ -2628,7 +2648,7 @@
       </c>
       <c r="W17" s="10"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23">
       <c r="A18" s="9">
         <v>16</v>
       </c>
@@ -2654,7 +2674,7 @@
       </c>
       <c r="W18" s="10"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23">
       <c r="A19" s="9">
         <v>17</v>
       </c>
@@ -2683,7 +2703,7 @@
       </c>
       <c r="W19" s="10"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23">
       <c r="A20" s="9">
         <v>18</v>
       </c>
@@ -2707,7 +2727,7 @@
       </c>
       <c r="W20" s="10"/>
     </row>
-    <row r="21" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" ht="60">
       <c r="A21" s="9">
         <v>19</v>
       </c>
@@ -2742,7 +2762,7 @@
       </c>
       <c r="W21" s="10"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23">
       <c r="A22" s="9">
         <v>20</v>
       </c>
@@ -2768,7 +2788,7 @@
       </c>
       <c r="W22" s="10"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23">
       <c r="A23" s="9">
         <v>21</v>
       </c>
@@ -2797,7 +2817,7 @@
       </c>
       <c r="W23" s="10"/>
     </row>
-    <row r="24" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" ht="45">
       <c r="A24" s="9">
         <v>22</v>
       </c>
@@ -2834,7 +2854,7 @@
       </c>
       <c r="W24" s="10"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23">
       <c r="A25" s="9">
         <v>23</v>
       </c>
@@ -2860,7 +2880,7 @@
       </c>
       <c r="W25" s="10"/>
     </row>
-    <row r="26" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" ht="60">
       <c r="A26" s="13" t="s">
         <v>31</v>
       </c>
@@ -2898,7 +2918,7 @@
       </c>
       <c r="W26" s="10"/>
     </row>
-    <row r="27" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" ht="30">
       <c r="A27" s="14" t="s">
         <v>32</v>
       </c>
@@ -2925,7 +2945,7 @@
       </c>
       <c r="W27" s="10"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23">
       <c r="A28" s="14" t="s">
         <v>34</v>
       </c>
@@ -2952,7 +2972,7 @@
       </c>
       <c r="W28" s="10"/>
     </row>
-    <row r="29" spans="1:23" ht="195" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" ht="195">
       <c r="A29" s="14" t="s">
         <v>36</v>
       </c>
@@ -2982,7 +3002,7 @@
       </c>
       <c r="W29" s="10"/>
     </row>
-    <row r="30" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" ht="30">
       <c r="A30" s="14" t="s">
         <v>38</v>
       </c>
@@ -3009,7 +3029,7 @@
       </c>
       <c r="W30" s="10"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23">
       <c r="A31" s="9">
         <v>24</v>
       </c>
@@ -3033,7 +3053,7 @@
       </c>
       <c r="W31" s="10"/>
     </row>
-    <row r="32" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" ht="15.75" thickBot="1">
       <c r="A32" s="20"/>
       <c r="B32" s="15"/>
       <c r="C32" s="16"/>
@@ -3070,4 +3090,687 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:W32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" style="18" customWidth="1"/>
+    <col min="2" max="2" width="49.140625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="11"/>
+    <col min="4" max="4" width="65" style="11" customWidth="1"/>
+    <col min="5" max="5" width="15" style="11" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="11"/>
+    <col min="7" max="7" width="58.28515625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="105" style="11" customWidth="1"/>
+    <col min="11" max="11" width="23" style="11" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" style="11" customWidth="1"/>
+    <col min="13" max="13" width="45.28515625" style="11" customWidth="1"/>
+    <col min="14" max="20" width="9.140625" style="11"/>
+    <col min="21" max="21" width="9.140625" style="11" customWidth="1"/>
+    <col min="22" max="22" width="62.140625" style="11" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" style="11" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="64"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="65"/>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="53"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="1"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="54"/>
+      <c r="W2" s="8"/>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="1"/>
+      <c r="H3" s="19"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="1"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="1"/>
+      <c r="W3" s="10"/>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="1"/>
+      <c r="H4" s="19"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="1"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="1"/>
+      <c r="W4" s="10"/>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5" s="9">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="1"/>
+      <c r="H5" s="19"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="1"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="1"/>
+      <c r="W5" s="10"/>
+    </row>
+    <row r="6" spans="1:23" ht="30">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="1"/>
+      <c r="H6" s="19"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="1"/>
+      <c r="T6" s="10"/>
+      <c r="W6" s="10"/>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7" s="9">
+        <v>5</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="1"/>
+      <c r="H7" s="19"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="1"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="1"/>
+      <c r="W7" s="10"/>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" s="9">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="1"/>
+      <c r="H8" s="19"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="1"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="1"/>
+      <c r="W8" s="10"/>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9" s="9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="1"/>
+      <c r="H9" s="19"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="1"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="1"/>
+      <c r="W9" s="10"/>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="1"/>
+      <c r="H10" s="19"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="1"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="1"/>
+      <c r="W10" s="10"/>
+    </row>
+    <row r="11" spans="1:23" ht="45">
+      <c r="A11" s="9">
+        <v>9</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="1"/>
+      <c r="H11" s="19"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="1"/>
+      <c r="T11" s="10"/>
+      <c r="W11" s="10"/>
+    </row>
+    <row r="12" spans="1:23" ht="45">
+      <c r="A12" s="9">
+        <v>10</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="1"/>
+      <c r="H12" s="19"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="1"/>
+      <c r="T12" s="10"/>
+      <c r="W12" s="10"/>
+    </row>
+    <row r="13" spans="1:23" ht="30">
+      <c r="A13" s="9">
+        <v>11</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="1"/>
+      <c r="H13" s="19"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="1"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="1"/>
+      <c r="W13" s="10"/>
+    </row>
+    <row r="14" spans="1:23" ht="45">
+      <c r="A14" s="9">
+        <v>12</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="1"/>
+      <c r="H14" s="19"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="1"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="1"/>
+      <c r="W14" s="10"/>
+    </row>
+    <row r="15" spans="1:23" ht="123.75" customHeight="1">
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="1"/>
+      <c r="H15" s="19"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="1"/>
+      <c r="T15" s="10"/>
+      <c r="W15" s="10"/>
+    </row>
+    <row r="16" spans="1:23" ht="45">
+      <c r="A16" s="9">
+        <v>14</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="1"/>
+      <c r="H16" s="19"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="1"/>
+      <c r="T16" s="10"/>
+      <c r="W16" s="10"/>
+    </row>
+    <row r="17" spans="1:23">
+      <c r="A17" s="9">
+        <v>15</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="1"/>
+      <c r="H17" s="19"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="1"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="1"/>
+      <c r="W17" s="10"/>
+    </row>
+    <row r="18" spans="1:23">
+      <c r="A18" s="9">
+        <v>16</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="1"/>
+      <c r="H18" s="19"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="1"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="1"/>
+      <c r="W18" s="10"/>
+    </row>
+    <row r="19" spans="1:23">
+      <c r="A19" s="9">
+        <v>17</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="1"/>
+      <c r="H19" s="19"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="1"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="1"/>
+      <c r="W19" s="10"/>
+    </row>
+    <row r="20" spans="1:23">
+      <c r="A20" s="9">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="1"/>
+      <c r="H20" s="19"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="1"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="1"/>
+      <c r="W20" s="10"/>
+    </row>
+    <row r="21" spans="1:23">
+      <c r="A21" s="9">
+        <v>19</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="1"/>
+      <c r="H21" s="19"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="1"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="1"/>
+      <c r="W21" s="10"/>
+    </row>
+    <row r="22" spans="1:23">
+      <c r="A22" s="9">
+        <v>20</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="1"/>
+      <c r="H22" s="19"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="1"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="1"/>
+      <c r="W22" s="10"/>
+    </row>
+    <row r="23" spans="1:23">
+      <c r="A23" s="9">
+        <v>21</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="1"/>
+      <c r="H23" s="19"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="1"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="1"/>
+      <c r="W23" s="10"/>
+    </row>
+    <row r="24" spans="1:23">
+      <c r="A24" s="9">
+        <v>22</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="1"/>
+      <c r="H24" s="19"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="1"/>
+      <c r="T24" s="10"/>
+      <c r="W24" s="10"/>
+    </row>
+    <row r="25" spans="1:23">
+      <c r="A25" s="9">
+        <v>23</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="1"/>
+      <c r="H25" s="19"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="1"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="1"/>
+      <c r="W25" s="10"/>
+    </row>
+    <row r="26" spans="1:23" ht="30">
+      <c r="A26" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E26" s="12"/>
+      <c r="F26" s="1"/>
+      <c r="H26" s="19"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="1"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="1"/>
+      <c r="W26" s="10"/>
+    </row>
+    <row r="27" spans="1:23" ht="30">
+      <c r="A27" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="1"/>
+      <c r="H27" s="19"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="1"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="1"/>
+      <c r="W27" s="10"/>
+    </row>
+    <row r="28" spans="1:23">
+      <c r="A28" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="1"/>
+      <c r="H28" s="19"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="1"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="1"/>
+      <c r="W28" s="10"/>
+    </row>
+    <row r="29" spans="1:23" ht="30">
+      <c r="A29" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="1"/>
+      <c r="H29" s="19"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="1"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="1"/>
+      <c r="W29" s="10"/>
+    </row>
+    <row r="30" spans="1:23" ht="30">
+      <c r="A30" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="1"/>
+      <c r="H30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="1"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="1"/>
+      <c r="W30" s="10"/>
+    </row>
+    <row r="31" spans="1:23">
+      <c r="A31" s="9">
+        <v>24</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="1"/>
+      <c r="H31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="1"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="1"/>
+      <c r="W31" s="10"/>
+    </row>
+    <row r="32" spans="1:23" ht="15.75" thickBot="1">
+      <c r="A32" s="20"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="15"/>
+      <c r="U32" s="16"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="U1:W1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Release 0.10.0 version change and testing protocol
</commit_message>
<xml_diff>
--- a/QualiMasterApplication/documentation/Testing Protocol.xlsx
+++ b/QualiMasterApplication/documentation/Testing Protocol.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13290" windowHeight="9285" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13290" windowHeight="9285" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="0.8.5" sheetId="4" r:id="rId1"/>
     <sheet name="0.9.0" sheetId="1" r:id="rId2"/>
     <sheet name="0.9.5" sheetId="6" r:id="rId3"/>
+    <sheet name="0.10.0" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="136">
   <si>
     <t>Result</t>
   </si>
@@ -431,6 +432,18 @@
   </si>
   <si>
     <t>Roman: 0.9.5 win 64-bit (2016-04-21), Windows 7 64-bit, Java jdk1.8.0_74 64-bit with QM2 model</t>
+  </si>
+  <si>
+    <t>Roman: 0.10.0 win 64-bit (2016-06-08), Windows 7 64-bit, Java jdk1.8.0_74 64-bit with ConfModel</t>
+  </si>
+  <si>
+    <t>Need to select another property field to make editor dirty</t>
+  </si>
+  <si>
+    <t>AlgorithmFamily is not shown in the Algorithm section after Algorithm is assigned to it. Only after restart.</t>
+  </si>
+  <si>
+    <t>after changing constraint from pipeline editor full qualified names are shown in the constraint</t>
   </si>
 </sst>
 </file>
@@ -590,7 +603,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -759,6 +772,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1363,21 +1379,21 @@
     <row r="1" spans="1:11">
       <c r="A1" s="26"/>
       <c r="B1" s="27"/>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="59"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="58" t="s">
+      <c r="D1" s="60"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="59"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="61" t="s">
+      <c r="G1" s="60"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="29" t="s">
@@ -1568,10 +1584,10 @@
       </c>
       <c r="G8" s="39"/>
       <c r="H8"/>
-      <c r="I8" s="62" t="s">
+      <c r="I8" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="63" t="s">
+      <c r="J8" s="64" t="s">
         <v>65</v>
       </c>
       <c r="K8"/>
@@ -1599,8 +1615,8 @@
         <v>68</v>
       </c>
       <c r="H9"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="63"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="64"/>
       <c r="K9" t="s">
         <v>69</v>
       </c>
@@ -2119,37 +2135,37 @@
     <row r="1" spans="1:23">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="64" t="s">
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="65"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="65" t="s">
+      <c r="G1" s="66"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="66" t="s">
         <v>125</v>
       </c>
-      <c r="J1" s="65"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="64" t="s">
+      <c r="J1" s="66"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="65" t="s">
         <v>114</v>
       </c>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
       <c r="Q1" s="55"/>
       <c r="R1" s="55"/>
       <c r="S1" s="55"/>
       <c r="T1" s="3"/>
-      <c r="U1" s="64" t="s">
+      <c r="U1" s="65" t="s">
         <v>117</v>
       </c>
-      <c r="V1" s="65"/>
-      <c r="W1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="67"/>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="4" t="s">
@@ -3102,7 +3118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -3134,29 +3150,29 @@
     <row r="1" spans="1:23">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="65" t="s">
         <v>131</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
       <c r="Q1" s="55"/>
       <c r="R1" s="55"/>
       <c r="S1" s="55"/>
       <c r="T1" s="3"/>
-      <c r="U1" s="64"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="66"/>
+      <c r="U1" s="65"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="67"/>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="4" t="s">
@@ -3782,4 +3798,684 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:W32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" style="18" customWidth="1"/>
+    <col min="2" max="2" width="49.140625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="11"/>
+    <col min="4" max="4" width="65" style="11" customWidth="1"/>
+    <col min="5" max="5" width="15" style="11" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="11"/>
+    <col min="7" max="7" width="58.28515625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="105" style="11" customWidth="1"/>
+    <col min="11" max="11" width="23" style="11" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" style="11" customWidth="1"/>
+    <col min="13" max="13" width="45.28515625" style="11" customWidth="1"/>
+    <col min="14" max="20" width="9.140625" style="11"/>
+    <col min="21" max="21" width="9.140625" style="11" customWidth="1"/>
+    <col min="22" max="22" width="62.140625" style="11" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" style="11" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="65"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="67"/>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="53"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="1"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="54"/>
+      <c r="W2" s="8"/>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="1"/>
+      <c r="H3" s="19"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="1"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="1"/>
+      <c r="W3" s="10"/>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="1"/>
+      <c r="H4" s="19"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="1"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="1"/>
+      <c r="W4" s="10"/>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5" s="9">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="1"/>
+      <c r="H5" s="19"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="1"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="1"/>
+      <c r="W5" s="10"/>
+    </row>
+    <row r="6" spans="1:23" ht="30">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="1"/>
+      <c r="H6" s="19"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="1"/>
+      <c r="T6" s="10"/>
+      <c r="W6" s="10"/>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7" s="9">
+        <v>5</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="1"/>
+      <c r="H7" s="19"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="1"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="1"/>
+      <c r="W7" s="10"/>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" s="9">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="1"/>
+      <c r="H8" s="19"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="1"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="1"/>
+      <c r="W8" s="10"/>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9" s="9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="1"/>
+      <c r="H9" s="19"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="1"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="1"/>
+      <c r="W9" s="10"/>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="1"/>
+      <c r="H10" s="19"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="1"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="1"/>
+      <c r="W10" s="10"/>
+    </row>
+    <row r="11" spans="1:23" ht="45">
+      <c r="A11" s="9">
+        <v>9</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="1"/>
+      <c r="H11" s="19"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="1"/>
+      <c r="T11" s="10"/>
+      <c r="W11" s="10"/>
+    </row>
+    <row r="12" spans="1:23" ht="45">
+      <c r="A12" s="9">
+        <v>10</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="1"/>
+      <c r="H12" s="19"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="1"/>
+      <c r="T12" s="10"/>
+      <c r="W12" s="10"/>
+    </row>
+    <row r="13" spans="1:23" ht="30">
+      <c r="A13" s="9">
+        <v>11</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="1"/>
+      <c r="H13" s="19"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="1"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="1"/>
+      <c r="W13" s="10"/>
+    </row>
+    <row r="14" spans="1:23" ht="45">
+      <c r="A14" s="9">
+        <v>12</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="1"/>
+      <c r="H14" s="19"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="1"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="1"/>
+      <c r="W14" s="10"/>
+    </row>
+    <row r="15" spans="1:23" ht="55.5" customHeight="1">
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="1"/>
+      <c r="H15" s="19"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="1"/>
+      <c r="T15" s="10"/>
+      <c r="W15" s="10"/>
+    </row>
+    <row r="16" spans="1:23" ht="45">
+      <c r="A16" s="9">
+        <v>14</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="1"/>
+      <c r="H16" s="19"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="1"/>
+      <c r="T16" s="10"/>
+      <c r="W16" s="10"/>
+    </row>
+    <row r="17" spans="1:23">
+      <c r="A17" s="9">
+        <v>15</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="1"/>
+      <c r="H17" s="19"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="1"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="1"/>
+      <c r="W17" s="10"/>
+    </row>
+    <row r="18" spans="1:23">
+      <c r="A18" s="9">
+        <v>16</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="1"/>
+      <c r="H18" s="19"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="1"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="1"/>
+      <c r="W18" s="10"/>
+    </row>
+    <row r="19" spans="1:23">
+      <c r="A19" s="9">
+        <v>17</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="1"/>
+      <c r="H19" s="19"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="1"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="1"/>
+      <c r="W19" s="10"/>
+    </row>
+    <row r="20" spans="1:23">
+      <c r="A20" s="9">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="1"/>
+      <c r="H20" s="19"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="1"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="1"/>
+      <c r="W20" s="10"/>
+    </row>
+    <row r="21" spans="1:23" ht="30">
+      <c r="A21" s="9">
+        <v>19</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="1"/>
+      <c r="H21" s="19"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="1"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="1"/>
+      <c r="W21" s="10"/>
+    </row>
+    <row r="22" spans="1:23">
+      <c r="A22" s="9">
+        <v>20</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="1"/>
+      <c r="H22" s="19"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="1"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="1"/>
+      <c r="W22" s="10"/>
+    </row>
+    <row r="23" spans="1:23">
+      <c r="A23" s="9">
+        <v>21</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="1"/>
+      <c r="H23" s="19"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="1"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="1"/>
+      <c r="W23" s="10"/>
+    </row>
+    <row r="24" spans="1:23">
+      <c r="A24" s="9">
+        <v>22</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="1"/>
+      <c r="H24" s="19"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="1"/>
+      <c r="T24" s="10"/>
+      <c r="W24" s="10"/>
+    </row>
+    <row r="25" spans="1:23">
+      <c r="A25" s="9">
+        <v>23</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="1"/>
+      <c r="H25" s="19"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="1"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="1"/>
+      <c r="W25" s="10"/>
+    </row>
+    <row r="26" spans="1:23">
+      <c r="A26" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="12"/>
+      <c r="F26" s="1"/>
+      <c r="H26" s="19"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="1"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="1"/>
+      <c r="W26" s="10"/>
+    </row>
+    <row r="27" spans="1:23" ht="30">
+      <c r="A27" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="1"/>
+      <c r="H27" s="19"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="1"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="1"/>
+      <c r="W27" s="10"/>
+    </row>
+    <row r="28" spans="1:23">
+      <c r="A28" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="1"/>
+      <c r="H28" s="19"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="1"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="1"/>
+      <c r="W28" s="10"/>
+    </row>
+    <row r="29" spans="1:23" ht="30">
+      <c r="A29" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="1"/>
+      <c r="H29" s="19"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="1"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="1"/>
+      <c r="W29" s="10"/>
+    </row>
+    <row r="30" spans="1:23" ht="30">
+      <c r="A30" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="1"/>
+      <c r="H30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="1"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="1"/>
+      <c r="W30" s="10"/>
+    </row>
+    <row r="31" spans="1:23">
+      <c r="A31" s="9">
+        <v>24</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="1"/>
+      <c r="H31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="1"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="1"/>
+      <c r="W31" s="10"/>
+    </row>
+    <row r="32" spans="1:23" ht="15.75" thickBot="1">
+      <c r="A32" s="20"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="15"/>
+      <c r="U32" s="16"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="U1:W1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Version update and test protocol
</commit_message>
<xml_diff>
--- a/QualiMasterApplication/documentation/Testing Protocol.xlsx
+++ b/QualiMasterApplication/documentation/Testing Protocol.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13290" windowHeight="9285" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13290" windowHeight="9285" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="0.8.5" sheetId="4" r:id="rId1"/>
     <sheet name="0.9.0" sheetId="1" r:id="rId2"/>
     <sheet name="0.9.5" sheetId="6" r:id="rId3"/>
     <sheet name="0.10.0" sheetId="8" r:id="rId4"/>
+    <sheet name="0.10.5" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="143">
   <si>
     <t>Result</t>
   </si>
@@ -444,6 +445,27 @@
   </si>
   <si>
     <t>after changing constraint from pipeline editor full qualified names are shown in the constraint</t>
+  </si>
+  <si>
+    <t>Artifact selected, but editor is not set dirty</t>
+  </si>
+  <si>
+    <t>HardwareAlgorithm and SubPipelineAlgorithm not tested</t>
+  </si>
+  <si>
+    <t>For Algorithms error- eu/qualimaster/observables/Imeasurable after selecting class; same for Sink and Source</t>
+  </si>
+  <si>
+    <t>was not able to delete FamilyElement and algorithm, after restart app crashed with unknown elements</t>
+  </si>
+  <si>
+    <t>It is possible to clone FamilyElement in Algoprithms, and it appears only in Algorithms, not under Families</t>
+  </si>
+  <si>
+    <t>adding name == "roman" eror name is unknow, same for latency == 1</t>
+  </si>
+  <si>
+    <t>Roman: 0.10.5 win 64-bit (2016-07-01), Windows 7 64-bit, Java jdk1.8.0_74 64-bit with ConfModel</t>
   </si>
 </sst>
 </file>
@@ -603,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -803,6 +825,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -925,7 +950,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -945,7 +970,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -980,7 +1005,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1000,7 +1025,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1035,7 +1060,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1055,7 +1080,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -3804,8 +3829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
@@ -4478,4 +4503,693 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:W32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" style="18" customWidth="1"/>
+    <col min="2" max="2" width="49.140625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="11"/>
+    <col min="4" max="4" width="65" style="11" customWidth="1"/>
+    <col min="5" max="5" width="15" style="11" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="11"/>
+    <col min="7" max="7" width="58.28515625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="105" style="11" customWidth="1"/>
+    <col min="11" max="11" width="23" style="11" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" style="11" customWidth="1"/>
+    <col min="13" max="13" width="45.28515625" style="11" customWidth="1"/>
+    <col min="14" max="20" width="9.140625" style="11"/>
+    <col min="21" max="21" width="9.140625" style="11" customWidth="1"/>
+    <col min="22" max="22" width="62.140625" style="11" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" style="11" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="65" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="65"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="67"/>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="53"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="1"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="54"/>
+      <c r="W2" s="8"/>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="1"/>
+      <c r="H3" s="19"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="1"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="1"/>
+      <c r="W3" s="10"/>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="1"/>
+      <c r="H4" s="19"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="1"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="1"/>
+      <c r="W4" s="10"/>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5" s="9">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="1"/>
+      <c r="H5" s="19"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="1"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="1"/>
+      <c r="W5" s="10"/>
+    </row>
+    <row r="6" spans="1:23" ht="30">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="1"/>
+      <c r="H6" s="19"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="1"/>
+      <c r="T6" s="10"/>
+      <c r="W6" s="10"/>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7" s="9">
+        <v>5</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="1"/>
+      <c r="H7" s="19"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="1"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="1"/>
+      <c r="W7" s="10"/>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" s="9">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="1"/>
+      <c r="H8" s="19"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="1"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="1"/>
+      <c r="W8" s="10"/>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9" s="9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="1"/>
+      <c r="H9" s="19"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="1"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="1"/>
+      <c r="W9" s="10"/>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="1"/>
+      <c r="H10" s="19"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="1"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="1"/>
+      <c r="W10" s="10"/>
+    </row>
+    <row r="11" spans="1:23" ht="45">
+      <c r="A11" s="9">
+        <v>9</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="1"/>
+      <c r="H11" s="19"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="1"/>
+      <c r="T11" s="10"/>
+      <c r="W11" s="10"/>
+    </row>
+    <row r="12" spans="1:23" ht="45">
+      <c r="A12" s="9">
+        <v>10</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="1"/>
+      <c r="H12" s="19"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="1"/>
+      <c r="T12" s="10"/>
+      <c r="W12" s="10"/>
+    </row>
+    <row r="13" spans="1:23" ht="30">
+      <c r="A13" s="9">
+        <v>11</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="1"/>
+      <c r="H13" s="19"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="1"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="1"/>
+      <c r="W13" s="10"/>
+    </row>
+    <row r="14" spans="1:23" ht="45">
+      <c r="A14" s="9">
+        <v>12</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="1"/>
+      <c r="H14" s="19"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="1"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="1"/>
+      <c r="W14" s="10"/>
+    </row>
+    <row r="15" spans="1:23" ht="55.5" customHeight="1">
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="1"/>
+      <c r="H15" s="19"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="1"/>
+      <c r="T15" s="10"/>
+      <c r="W15" s="10"/>
+    </row>
+    <row r="16" spans="1:23" ht="45">
+      <c r="A16" s="9">
+        <v>14</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="1"/>
+      <c r="H16" s="19"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="1"/>
+      <c r="T16" s="10"/>
+      <c r="W16" s="10"/>
+    </row>
+    <row r="17" spans="1:23">
+      <c r="A17" s="9">
+        <v>15</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="1"/>
+      <c r="H17" s="19"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="1"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="1"/>
+      <c r="W17" s="10"/>
+    </row>
+    <row r="18" spans="1:23">
+      <c r="A18" s="9">
+        <v>16</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="1"/>
+      <c r="H18" s="19"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="1"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="1"/>
+      <c r="W18" s="10"/>
+    </row>
+    <row r="19" spans="1:23">
+      <c r="A19" s="9">
+        <v>17</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="1"/>
+      <c r="H19" s="19"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="1"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="1"/>
+      <c r="W19" s="10"/>
+    </row>
+    <row r="20" spans="1:23">
+      <c r="A20" s="9">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="1"/>
+      <c r="H20" s="19"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="1"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="1"/>
+      <c r="W20" s="10"/>
+    </row>
+    <row r="21" spans="1:23">
+      <c r="A21" s="9">
+        <v>19</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="1"/>
+      <c r="H21" s="19"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="1"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="1"/>
+      <c r="W21" s="10"/>
+    </row>
+    <row r="22" spans="1:23">
+      <c r="A22" s="9">
+        <v>20</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="1"/>
+      <c r="H22" s="19"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="1"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="1"/>
+      <c r="W22" s="10"/>
+    </row>
+    <row r="23" spans="1:23">
+      <c r="A23" s="9">
+        <v>21</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="1"/>
+      <c r="H23" s="19"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="1"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="1"/>
+      <c r="W23" s="10"/>
+    </row>
+    <row r="24" spans="1:23">
+      <c r="A24" s="9">
+        <v>22</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="1"/>
+      <c r="H24" s="19"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="1"/>
+      <c r="T24" s="10"/>
+      <c r="W24" s="10"/>
+    </row>
+    <row r="25" spans="1:23">
+      <c r="A25" s="9">
+        <v>23</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="1"/>
+      <c r="H25" s="19"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="1"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="1"/>
+      <c r="W25" s="10"/>
+    </row>
+    <row r="26" spans="1:23">
+      <c r="A26" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="12"/>
+      <c r="F26" s="1"/>
+      <c r="H26" s="19"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="1"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="1"/>
+      <c r="W26" s="10"/>
+    </row>
+    <row r="27" spans="1:23" ht="30">
+      <c r="A27" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="1"/>
+      <c r="H27" s="19"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="1"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="1"/>
+      <c r="W27" s="10"/>
+    </row>
+    <row r="28" spans="1:23">
+      <c r="A28" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="1"/>
+      <c r="H28" s="19"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="1"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="1"/>
+      <c r="W28" s="10"/>
+    </row>
+    <row r="29" spans="1:23" ht="30">
+      <c r="A29" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="1"/>
+      <c r="H29" s="19"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="1"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="1"/>
+      <c r="W29" s="10"/>
+    </row>
+    <row r="30" spans="1:23" ht="30">
+      <c r="A30" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="1"/>
+      <c r="H30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="1"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="1"/>
+      <c r="W30" s="10"/>
+    </row>
+    <row r="31" spans="1:23">
+      <c r="A31" s="9">
+        <v>24</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="1"/>
+      <c r="H31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="1"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="1"/>
+      <c r="W31" s="10"/>
+    </row>
+    <row r="32" spans="1:23" ht="15.75" thickBot="1">
+      <c r="A32" s="20"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="15"/>
+      <c r="U32" s="16"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="U1:W1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Testing protocol for 0.10.5 release
</commit_message>
<xml_diff>
--- a/QualiMasterApplication/documentation/Testing Protocol.xlsx
+++ b/QualiMasterApplication/documentation/Testing Protocol.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="145">
   <si>
     <t>Result</t>
   </si>
@@ -447,31 +447,31 @@
     <t>after changing constraint from pipeline editor full qualified names are shown in the constraint</t>
   </si>
   <si>
-    <t>Artifact selected, but editor is not set dirty</t>
-  </si>
-  <si>
     <t>HardwareAlgorithm and SubPipelineAlgorithm not tested</t>
   </si>
   <si>
-    <t>For Algorithms error- eu/qualimaster/observables/Imeasurable after selecting class; same for Sink and Source</t>
-  </si>
-  <si>
-    <t>was not able to delete FamilyElement and algorithm, after restart app crashed with unknown elements</t>
-  </si>
-  <si>
-    <t>It is possible to clone FamilyElement in Algoprithms, and it appears only in Algorithms, not under Families</t>
-  </si>
-  <si>
-    <t>adding name == "roman" eror name is unknow, same for latency == 1</t>
-  </si>
-  <si>
-    <t>Roman: 0.10.5 win 64-bit (2016-07-01), Windows 7 64-bit, Java jdk1.8.0_74 64-bit with ConfModel</t>
-  </si>
-  <si>
-    <t>no more error, but nothing appears after presing Browse at class</t>
-  </si>
-  <si>
-    <t>still exists</t>
+    <t>Roman: 0.10.5 win 64-bit (2016-07-08), Windows 7 64-bit, Java jdk1.8.0_74 64-bit with ConfModel</t>
+  </si>
+  <si>
+    <t>When Algorithm added to FamilyElement, FE appears under Algorithms only after application restart.</t>
+  </si>
+  <si>
+    <t>For Algorithms error- eu/qualimaster/observables/Imeasurable after selecting class; same for Source. Sink works.</t>
+  </si>
+  <si>
+    <t>Deleted FE disapears under Algorithm only after app restart</t>
+  </si>
+  <si>
+    <t>It is possible to clone FamilyElement in Algoprithms, and it appears only in Algorithms, not under Families (appears under Families after app restart)</t>
+  </si>
+  <si>
+    <t>Now 6 errors found as new pipeline added</t>
+  </si>
+  <si>
+    <t>New error msg with "flow end"</t>
+  </si>
+  <si>
+    <t>no testDMPip pipeline in ConfModel</t>
   </si>
 </sst>
 </file>
@@ -501,7 +501,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -535,12 +535,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -637,7 +631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -840,12 +834,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -968,7 +956,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -988,7 +976,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1023,7 +1011,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1043,7 +1031,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1078,7 +1066,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1098,7 +1086,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -4528,10 +4516,10 @@
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4560,7 +4548,7 @@
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="66" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D1" s="67"/>
       <c r="E1" s="68"/>
@@ -4731,15 +4719,10 @@
       <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="E9" s="69" t="s">
-        <v>115</v>
-      </c>
+      <c r="C9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="10"/>
       <c r="F9" s="1"/>
       <c r="H9" s="19"/>
       <c r="K9" s="10"/>
@@ -4774,11 +4757,11 @@
       <c r="B11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="58" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="1"/>
@@ -4798,6 +4781,9 @@
       <c r="C12" s="11" t="s">
         <v>40</v>
       </c>
+      <c r="D12" s="11" t="s">
+        <v>138</v>
+      </c>
       <c r="E12" s="10"/>
       <c r="F12" s="1"/>
       <c r="H12" s="19"/>
@@ -4806,7 +4792,7 @@
       <c r="T12" s="10"/>
       <c r="W12" s="10"/>
     </row>
-    <row r="13" spans="1:23" ht="75">
+    <row r="13" spans="1:23" ht="30">
       <c r="A13" s="9">
         <v>11</v>
       </c>
@@ -4817,11 +4803,9 @@
         <v>41</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="E13" s="70" t="s">
-        <v>143</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="E13" s="10"/>
       <c r="F13" s="1"/>
       <c r="H13" s="19"/>
       <c r="K13" s="10"/>
@@ -4856,15 +4840,13 @@
       <c r="B15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>41</v>
+      <c r="C15" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="E15" s="69" t="s">
-        <v>115</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="E15" s="10"/>
       <c r="F15" s="1"/>
       <c r="H15" s="19"/>
       <c r="K15" s="10"/>
@@ -4879,11 +4861,11 @@
       <c r="B16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="1"/>
@@ -4976,15 +4958,10 @@
       <c r="B21" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="E21" s="70" t="s">
-        <v>144</v>
-      </c>
+      <c r="C21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="10"/>
       <c r="F21" s="1"/>
       <c r="H21" s="19"/>
       <c r="K21" s="10"/>
@@ -5097,6 +5074,9 @@
       <c r="C27" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="D27" s="11" t="s">
+        <v>142</v>
+      </c>
       <c r="E27" s="10"/>
       <c r="F27" s="1"/>
       <c r="H27" s="19"/>
@@ -5135,6 +5115,9 @@
       <c r="C29" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="D29" s="11" t="s">
+        <v>143</v>
+      </c>
       <c r="E29" s="10"/>
       <c r="F29" s="1"/>
       <c r="H29" s="19"/>
@@ -5151,8 +5134,9 @@
       <c r="B30" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>40</v>
+      <c r="C30" s="1"/>
+      <c r="D30" s="11" t="s">
+        <v>144</v>
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="1"/>

</xml_diff>

<commit_message>
First changes for release 0.11.0
However, I wait for a blocking bug fix from Patrik.
</commit_message>
<xml_diff>
--- a/QualiMasterApplication/documentation/Testing Protocol.xlsx
+++ b/QualiMasterApplication/documentation/Testing Protocol.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13290" windowHeight="9285" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13290" windowHeight="9285" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="0.8.5" sheetId="4" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="0.9.5" sheetId="6" r:id="rId3"/>
     <sheet name="0.10.0" sheetId="8" r:id="rId4"/>
     <sheet name="0.10.5" sheetId="9" r:id="rId5"/>
+    <sheet name="0.11.0" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="151">
   <si>
     <t>Result</t>
   </si>
@@ -473,12 +474,30 @@
   <si>
     <t>no testDMPip pipeline in ConfModel</t>
   </si>
+  <si>
+    <t>Sascha: 0.11.0 win 64-bit (2016-10-28), Windows 7 64-bit, Java jdk1.8.0_102 64-bit with QM2.devel Model</t>
+  </si>
+  <si>
+    <t>Also downloads the archive in offline mode (I had no cached information in fresh workspace available)</t>
+  </si>
+  <si>
+    <t>After selecting a class, the app is throwing an error (cf. 1st screenshot). I expect a maven dependency problem behin this problem</t>
+  </si>
+  <si>
+    <t>partially</t>
+  </si>
+  <si>
+    <t>Works but cloned algorithms are not selected in their family (Issue #92).</t>
+  </si>
+  <si>
+    <t>Filed new Issue #133</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -631,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -835,9 +854,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -956,7 +987,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -976,7 +1007,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1011,7 +1042,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1031,7 +1062,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1066,7 +1097,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1086,7 +1117,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1100,10 +1131,53 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>16750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1286974</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>723899</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4076699" y="2112250"/>
+          <a:ext cx="4620725" cy="1850149"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1141,7 +1215,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1175,6 +1249,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1209,9 +1284,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1384,14 +1460,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="52" customWidth="1"/>
     <col min="2" max="2" width="49.140625" style="28" customWidth="1"/>
@@ -1407,7 +1483,7 @@
     <col min="12" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="26"/>
       <c r="B1" s="27"/>
       <c r="C1" s="60" t="s">
@@ -1426,7 +1502,7 @@
       <c r="J1" s="63"/>
       <c r="K1" s="63"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>3</v>
       </c>
@@ -1461,7 +1537,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30">
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="36">
         <v>1</v>
       </c>
@@ -1490,7 +1566,7 @@
       </c>
       <c r="K3"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="36">
         <v>2</v>
       </c>
@@ -1513,7 +1589,7 @@
       <c r="J4"/>
       <c r="K4"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="36">
         <v>3</v>
       </c>
@@ -1536,7 +1612,7 @@
       <c r="J5"/>
       <c r="K5"/>
     </row>
-    <row r="6" spans="1:11" ht="81.75" customHeight="1">
+    <row r="6" spans="1:11" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36">
         <v>4</v>
       </c>
@@ -1567,7 +1643,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="30">
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="36">
         <v>5</v>
       </c>
@@ -1594,7 +1670,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30">
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="36">
         <v>6</v>
       </c>
@@ -1623,7 +1699,7 @@
       </c>
       <c r="K8"/>
     </row>
-    <row r="9" spans="1:11" ht="30">
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="36">
         <v>7</v>
       </c>
@@ -1652,7 +1728,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="30">
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="36">
         <v>8</v>
       </c>
@@ -1679,7 +1755,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="45">
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="36">
         <v>9</v>
       </c>
@@ -1702,7 +1778,7 @@
       <c r="J11"/>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:11" ht="45">
+    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="36">
         <v>10</v>
       </c>
@@ -1733,7 +1809,7 @@
       <c r="J12"/>
       <c r="K12"/>
     </row>
-    <row r="13" spans="1:11" ht="45">
+    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="36">
         <v>11</v>
       </c>
@@ -1756,7 +1832,7 @@
       <c r="J13"/>
       <c r="K13"/>
     </row>
-    <row r="14" spans="1:11" ht="60">
+    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="36">
         <v>12</v>
       </c>
@@ -1783,7 +1859,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="45">
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="36">
         <v>13</v>
       </c>
@@ -1806,7 +1882,7 @@
       <c r="J15"/>
       <c r="K15"/>
     </row>
-    <row r="16" spans="1:11" ht="30">
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="36">
         <v>14</v>
       </c>
@@ -1837,7 +1913,7 @@
       <c r="J16"/>
       <c r="K16"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="36">
         <v>15</v>
       </c>
@@ -1860,7 +1936,7 @@
       <c r="J17"/>
       <c r="K17"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="36">
         <v>16</v>
       </c>
@@ -1883,7 +1959,7 @@
       <c r="J18"/>
       <c r="K18"/>
     </row>
-    <row r="19" spans="1:11" ht="30">
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="36">
         <v>17</v>
       </c>
@@ -1910,7 +1986,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="120">
+    <row r="20" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="36">
         <v>18</v>
       </c>
@@ -1943,7 +2019,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="36">
         <v>19</v>
       </c>
@@ -1966,7 +2042,7 @@
       <c r="J21"/>
       <c r="K21"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="36">
         <v>20</v>
       </c>
@@ -1989,7 +2065,7 @@
       <c r="J22"/>
       <c r="K22"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="36">
         <v>21</v>
       </c>
@@ -2012,7 +2088,7 @@
       <c r="J23"/>
       <c r="K23"/>
     </row>
-    <row r="24" spans="1:11" ht="30">
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="46" t="s">
         <v>89</v>
       </c>
@@ -2043,7 +2119,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="30">
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="47" t="s">
         <v>94</v>
       </c>
@@ -2066,7 +2142,7 @@
       <c r="J25"/>
       <c r="K25"/>
     </row>
-    <row r="26" spans="1:11" ht="30">
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="47" t="s">
         <v>95</v>
       </c>
@@ -2093,7 +2169,7 @@
       <c r="J26"/>
       <c r="K26"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1">
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="48">
         <v>22</v>
       </c>
@@ -2131,7 +2207,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2141,7 +2217,7 @@
       <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="18" customWidth="1"/>
     <col min="2" max="2" width="49.140625" style="11" customWidth="1"/>
@@ -2163,7 +2239,7 @@
     <col min="24" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="66" t="s">
@@ -2198,7 +2274,7 @@
       <c r="V1" s="67"/>
       <c r="W1" s="68"/>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -2244,7 +2320,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -2272,7 +2348,7 @@
       </c>
       <c r="W3" s="10"/>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -2298,7 +2374,7 @@
       </c>
       <c r="W4" s="10"/>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -2324,7 +2400,7 @@
       </c>
       <c r="W5" s="10"/>
     </row>
-    <row r="6" spans="1:23" ht="60">
+    <row r="6" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -2356,7 +2432,7 @@
       </c>
       <c r="W6" s="10"/>
     </row>
-    <row r="7" spans="1:23" ht="30">
+    <row r="7" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -2385,7 +2461,7 @@
       </c>
       <c r="W7" s="10"/>
     </row>
-    <row r="8" spans="1:23" ht="30">
+    <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -2414,7 +2490,7 @@
       </c>
       <c r="W8" s="10"/>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>7</v>
       </c>
@@ -2443,7 +2519,7 @@
       </c>
       <c r="W9" s="10"/>
     </row>
-    <row r="10" spans="1:23" ht="30">
+    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -2474,7 +2550,7 @@
       </c>
       <c r="W10" s="10"/>
     </row>
-    <row r="11" spans="1:23" ht="90">
+    <row r="11" spans="1:23" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -2503,7 +2579,7 @@
       </c>
       <c r="W11" s="10"/>
     </row>
-    <row r="12" spans="1:23" ht="45">
+    <row r="12" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
@@ -2543,7 +2619,7 @@
       </c>
       <c r="W12" s="10"/>
     </row>
-    <row r="13" spans="1:23" ht="30">
+    <row r="13" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>11</v>
       </c>
@@ -2582,7 +2658,7 @@
       </c>
       <c r="W13" s="10"/>
     </row>
-    <row r="14" spans="1:23" ht="45">
+    <row r="14" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
@@ -2611,7 +2687,7 @@
       </c>
       <c r="W14" s="10"/>
     </row>
-    <row r="15" spans="1:23" ht="123.75" customHeight="1">
+    <row r="15" spans="1:23" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>13</v>
       </c>
@@ -2646,7 +2722,7 @@
       </c>
       <c r="W15" s="10"/>
     </row>
-    <row r="16" spans="1:23" ht="60">
+    <row r="16" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>14</v>
       </c>
@@ -2675,7 +2751,7 @@
       </c>
       <c r="W16" s="10"/>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>15</v>
       </c>
@@ -2701,7 +2777,7 @@
       </c>
       <c r="W17" s="10"/>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>16</v>
       </c>
@@ -2727,7 +2803,7 @@
       </c>
       <c r="W18" s="10"/>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>17</v>
       </c>
@@ -2756,7 +2832,7 @@
       </c>
       <c r="W19" s="10"/>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>18</v>
       </c>
@@ -2780,7 +2856,7 @@
       </c>
       <c r="W20" s="10"/>
     </row>
-    <row r="21" spans="1:23" ht="60">
+    <row r="21" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>19</v>
       </c>
@@ -2815,7 +2891,7 @@
       </c>
       <c r="W21" s="10"/>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>20</v>
       </c>
@@ -2841,7 +2917,7 @@
       </c>
       <c r="W22" s="10"/>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>21</v>
       </c>
@@ -2870,7 +2946,7 @@
       </c>
       <c r="W23" s="10"/>
     </row>
-    <row r="24" spans="1:23" ht="45">
+    <row r="24" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>22</v>
       </c>
@@ -2907,7 +2983,7 @@
       </c>
       <c r="W24" s="10"/>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>23</v>
       </c>
@@ -2933,7 +3009,7 @@
       </c>
       <c r="W25" s="10"/>
     </row>
-    <row r="26" spans="1:23" ht="60">
+    <row r="26" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>31</v>
       </c>
@@ -2971,7 +3047,7 @@
       </c>
       <c r="W26" s="10"/>
     </row>
-    <row r="27" spans="1:23" ht="30">
+    <row r="27" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>32</v>
       </c>
@@ -2998,7 +3074,7 @@
       </c>
       <c r="W27" s="10"/>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>34</v>
       </c>
@@ -3025,7 +3101,7 @@
       </c>
       <c r="W28" s="10"/>
     </row>
-    <row r="29" spans="1:23" ht="195">
+    <row r="29" spans="1:23" ht="195" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>36</v>
       </c>
@@ -3055,7 +3131,7 @@
       </c>
       <c r="W29" s="10"/>
     </row>
-    <row r="30" spans="1:23" ht="30">
+    <row r="30" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>38</v>
       </c>
@@ -3082,7 +3158,7 @@
       </c>
       <c r="W30" s="10"/>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>24</v>
       </c>
@@ -3106,7 +3182,7 @@
       </c>
       <c r="W31" s="10"/>
     </row>
-    <row r="32" spans="1:23" ht="15.75" thickBot="1">
+    <row r="32" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="20"/>
       <c r="B32" s="15"/>
       <c r="C32" s="16"/>
@@ -3146,7 +3222,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3156,7 +3232,7 @@
       <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="18" customWidth="1"/>
     <col min="2" max="2" width="49.140625" style="11" customWidth="1"/>
@@ -3178,7 +3254,7 @@
     <col min="24" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="66" t="s">
@@ -3205,7 +3281,7 @@
       <c r="V1" s="67"/>
       <c r="W1" s="68"/>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -3233,7 +3309,7 @@
       <c r="V2" s="54"/>
       <c r="W2" s="8"/>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -3252,7 +3328,7 @@
       <c r="U3" s="1"/>
       <c r="W3" s="10"/>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -3271,7 +3347,7 @@
       <c r="U4" s="1"/>
       <c r="W4" s="10"/>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -3290,7 +3366,7 @@
       <c r="U5" s="1"/>
       <c r="W5" s="10"/>
     </row>
-    <row r="6" spans="1:23" ht="30">
+    <row r="6" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -3308,7 +3384,7 @@
       <c r="T6" s="10"/>
       <c r="W6" s="10"/>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -3327,7 +3403,7 @@
       <c r="U7" s="1"/>
       <c r="W7" s="10"/>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -3346,7 +3422,7 @@
       <c r="U8" s="1"/>
       <c r="W8" s="10"/>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>7</v>
       </c>
@@ -3365,7 +3441,7 @@
       <c r="U9" s="1"/>
       <c r="W9" s="10"/>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -3384,7 +3460,7 @@
       <c r="U10" s="1"/>
       <c r="W10" s="10"/>
     </row>
-    <row r="11" spans="1:23" ht="45">
+    <row r="11" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -3405,7 +3481,7 @@
       <c r="T11" s="10"/>
       <c r="W11" s="10"/>
     </row>
-    <row r="12" spans="1:23" ht="45">
+    <row r="12" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
@@ -3423,7 +3499,7 @@
       <c r="T12" s="10"/>
       <c r="W12" s="10"/>
     </row>
-    <row r="13" spans="1:23" ht="30">
+    <row r="13" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>11</v>
       </c>
@@ -3442,7 +3518,7 @@
       <c r="U13" s="1"/>
       <c r="W13" s="10"/>
     </row>
-    <row r="14" spans="1:23" ht="45">
+    <row r="14" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
@@ -3461,7 +3537,7 @@
       <c r="U14" s="1"/>
       <c r="W14" s="10"/>
     </row>
-    <row r="15" spans="1:23" ht="123.75" customHeight="1">
+    <row r="15" spans="1:23" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>13</v>
       </c>
@@ -3482,7 +3558,7 @@
       <c r="T15" s="10"/>
       <c r="W15" s="10"/>
     </row>
-    <row r="16" spans="1:23" ht="45">
+    <row r="16" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>14</v>
       </c>
@@ -3503,7 +3579,7 @@
       <c r="T16" s="10"/>
       <c r="W16" s="10"/>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>15</v>
       </c>
@@ -3522,7 +3598,7 @@
       <c r="U17" s="1"/>
       <c r="W17" s="10"/>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>16</v>
       </c>
@@ -3541,7 +3617,7 @@
       <c r="U18" s="1"/>
       <c r="W18" s="10"/>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>17</v>
       </c>
@@ -3560,7 +3636,7 @@
       <c r="U19" s="1"/>
       <c r="W19" s="10"/>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>18</v>
       </c>
@@ -3579,7 +3655,7 @@
       <c r="U20" s="1"/>
       <c r="W20" s="10"/>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>19</v>
       </c>
@@ -3598,7 +3674,7 @@
       <c r="U21" s="1"/>
       <c r="W21" s="10"/>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>20</v>
       </c>
@@ -3617,7 +3693,7 @@
       <c r="U22" s="1"/>
       <c r="W22" s="10"/>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>21</v>
       </c>
@@ -3636,7 +3712,7 @@
       <c r="U23" s="1"/>
       <c r="W23" s="10"/>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>22</v>
       </c>
@@ -3654,7 +3730,7 @@
       <c r="T24" s="10"/>
       <c r="W24" s="10"/>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>23</v>
       </c>
@@ -3673,7 +3749,7 @@
       <c r="U25" s="1"/>
       <c r="W25" s="10"/>
     </row>
-    <row r="26" spans="1:23" ht="30">
+    <row r="26" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>31</v>
       </c>
@@ -3695,7 +3771,7 @@
       <c r="U26" s="1"/>
       <c r="W26" s="10"/>
     </row>
-    <row r="27" spans="1:23" ht="30">
+    <row r="27" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>32</v>
       </c>
@@ -3714,7 +3790,7 @@
       <c r="U27" s="1"/>
       <c r="W27" s="10"/>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>34</v>
       </c>
@@ -3733,7 +3809,7 @@
       <c r="U28" s="1"/>
       <c r="W28" s="10"/>
     </row>
-    <row r="29" spans="1:23" ht="30">
+    <row r="29" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>36</v>
       </c>
@@ -3752,7 +3828,7 @@
       <c r="U29" s="1"/>
       <c r="W29" s="10"/>
     </row>
-    <row r="30" spans="1:23" ht="30">
+    <row r="30" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>38</v>
       </c>
@@ -3774,7 +3850,7 @@
       <c r="U30" s="1"/>
       <c r="W30" s="10"/>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>24</v>
       </c>
@@ -3793,7 +3869,7 @@
       <c r="U31" s="1"/>
       <c r="W31" s="10"/>
     </row>
-    <row r="32" spans="1:23" ht="15.75" thickBot="1">
+    <row r="32" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="20"/>
       <c r="B32" s="15"/>
       <c r="C32" s="16"/>
@@ -3832,7 +3908,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3842,7 +3918,7 @@
       <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="18" customWidth="1"/>
     <col min="2" max="2" width="49.140625" style="11" customWidth="1"/>
@@ -3864,7 +3940,7 @@
     <col min="24" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="66" t="s">
@@ -3891,7 +3967,7 @@
       <c r="V1" s="67"/>
       <c r="W1" s="68"/>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -3919,7 +3995,7 @@
       <c r="V2" s="54"/>
       <c r="W2" s="8"/>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -3938,7 +4014,7 @@
       <c r="U3" s="1"/>
       <c r="W3" s="10"/>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -3957,7 +4033,7 @@
       <c r="U4" s="1"/>
       <c r="W4" s="10"/>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -3976,7 +4052,7 @@
       <c r="U5" s="1"/>
       <c r="W5" s="10"/>
     </row>
-    <row r="6" spans="1:23" ht="30">
+    <row r="6" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -3994,7 +4070,7 @@
       <c r="T6" s="10"/>
       <c r="W6" s="10"/>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -4013,7 +4089,7 @@
       <c r="U7" s="1"/>
       <c r="W7" s="10"/>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -4032,7 +4108,7 @@
       <c r="U8" s="1"/>
       <c r="W8" s="10"/>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>7</v>
       </c>
@@ -4054,7 +4130,7 @@
       <c r="U9" s="1"/>
       <c r="W9" s="10"/>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -4073,7 +4149,7 @@
       <c r="U10" s="1"/>
       <c r="W10" s="10"/>
     </row>
-    <row r="11" spans="1:23" ht="45">
+    <row r="11" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -4091,7 +4167,7 @@
       <c r="T11" s="10"/>
       <c r="W11" s="10"/>
     </row>
-    <row r="12" spans="1:23" ht="45">
+    <row r="12" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
@@ -4112,7 +4188,7 @@
       <c r="T12" s="10"/>
       <c r="W12" s="10"/>
     </row>
-    <row r="13" spans="1:23" ht="30">
+    <row r="13" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>11</v>
       </c>
@@ -4131,7 +4207,7 @@
       <c r="U13" s="1"/>
       <c r="W13" s="10"/>
     </row>
-    <row r="14" spans="1:23" ht="45">
+    <row r="14" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
@@ -4150,7 +4226,7 @@
       <c r="U14" s="1"/>
       <c r="W14" s="10"/>
     </row>
-    <row r="15" spans="1:23" ht="55.5" customHeight="1">
+    <row r="15" spans="1:23" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>13</v>
       </c>
@@ -4168,7 +4244,7 @@
       <c r="T15" s="10"/>
       <c r="W15" s="10"/>
     </row>
-    <row r="16" spans="1:23" ht="45">
+    <row r="16" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>14</v>
       </c>
@@ -4186,7 +4262,7 @@
       <c r="T16" s="10"/>
       <c r="W16" s="10"/>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>15</v>
       </c>
@@ -4205,7 +4281,7 @@
       <c r="U17" s="1"/>
       <c r="W17" s="10"/>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>16</v>
       </c>
@@ -4224,7 +4300,7 @@
       <c r="U18" s="1"/>
       <c r="W18" s="10"/>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>17</v>
       </c>
@@ -4243,7 +4319,7 @@
       <c r="U19" s="1"/>
       <c r="W19" s="10"/>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>18</v>
       </c>
@@ -4262,7 +4338,7 @@
       <c r="U20" s="1"/>
       <c r="W20" s="10"/>
     </row>
-    <row r="21" spans="1:23" ht="30">
+    <row r="21" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>19</v>
       </c>
@@ -4284,7 +4360,7 @@
       <c r="U21" s="1"/>
       <c r="W21" s="10"/>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>20</v>
       </c>
@@ -4303,7 +4379,7 @@
       <c r="U22" s="1"/>
       <c r="W22" s="10"/>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>21</v>
       </c>
@@ -4322,7 +4398,7 @@
       <c r="U23" s="1"/>
       <c r="W23" s="10"/>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>22</v>
       </c>
@@ -4340,7 +4416,7 @@
       <c r="T24" s="10"/>
       <c r="W24" s="10"/>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>23</v>
       </c>
@@ -4359,7 +4435,7 @@
       <c r="U25" s="1"/>
       <c r="W25" s="10"/>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>31</v>
       </c>
@@ -4378,7 +4454,7 @@
       <c r="U26" s="1"/>
       <c r="W26" s="10"/>
     </row>
-    <row r="27" spans="1:23" ht="30">
+    <row r="27" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>32</v>
       </c>
@@ -4397,7 +4473,7 @@
       <c r="U27" s="1"/>
       <c r="W27" s="10"/>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>34</v>
       </c>
@@ -4416,7 +4492,7 @@
       <c r="U28" s="1"/>
       <c r="W28" s="10"/>
     </row>
-    <row r="29" spans="1:23" ht="30">
+    <row r="29" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>36</v>
       </c>
@@ -4435,7 +4511,7 @@
       <c r="U29" s="1"/>
       <c r="W29" s="10"/>
     </row>
-    <row r="30" spans="1:23" ht="30">
+    <row r="30" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>38</v>
       </c>
@@ -4454,7 +4530,7 @@
       <c r="U30" s="1"/>
       <c r="W30" s="10"/>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>24</v>
       </c>
@@ -4473,7 +4549,7 @@
       <c r="U31" s="1"/>
       <c r="W31" s="10"/>
     </row>
-    <row r="32" spans="1:23" ht="15.75" thickBot="1">
+    <row r="32" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="20"/>
       <c r="B32" s="15"/>
       <c r="C32" s="16"/>
@@ -4512,17 +4588,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="18" customWidth="1"/>
     <col min="2" max="2" width="49.140625" style="11" customWidth="1"/>
@@ -4544,7 +4620,7 @@
     <col min="24" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="66" t="s">
@@ -4571,7 +4647,7 @@
       <c r="V1" s="67"/>
       <c r="W1" s="68"/>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -4599,7 +4675,7 @@
       <c r="V2" s="54"/>
       <c r="W2" s="8"/>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -4618,7 +4694,7 @@
       <c r="U3" s="1"/>
       <c r="W3" s="10"/>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -4637,7 +4713,7 @@
       <c r="U4" s="1"/>
       <c r="W4" s="10"/>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -4656,7 +4732,7 @@
       <c r="U5" s="1"/>
       <c r="W5" s="10"/>
     </row>
-    <row r="6" spans="1:23" ht="30">
+    <row r="6" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -4674,7 +4750,7 @@
       <c r="T6" s="10"/>
       <c r="W6" s="10"/>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -4693,7 +4769,7 @@
       <c r="U7" s="1"/>
       <c r="W7" s="10"/>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -4712,7 +4788,7 @@
       <c r="U8" s="1"/>
       <c r="W8" s="10"/>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>7</v>
       </c>
@@ -4731,7 +4807,7 @@
       <c r="U9" s="1"/>
       <c r="W9" s="10"/>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -4750,7 +4826,7 @@
       <c r="U10" s="1"/>
       <c r="W10" s="10"/>
     </row>
-    <row r="11" spans="1:23" ht="45">
+    <row r="11" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -4771,7 +4847,7 @@
       <c r="T11" s="10"/>
       <c r="W11" s="10"/>
     </row>
-    <row r="12" spans="1:23" ht="45">
+    <row r="12" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
@@ -4792,7 +4868,7 @@
       <c r="T12" s="10"/>
       <c r="W12" s="10"/>
     </row>
-    <row r="13" spans="1:23" ht="30">
+    <row r="13" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>11</v>
       </c>
@@ -4814,7 +4890,7 @@
       <c r="U13" s="1"/>
       <c r="W13" s="10"/>
     </row>
-    <row r="14" spans="1:23" ht="45">
+    <row r="14" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
@@ -4833,7 +4909,7 @@
       <c r="U14" s="1"/>
       <c r="W14" s="10"/>
     </row>
-    <row r="15" spans="1:23" ht="55.5" customHeight="1">
+    <row r="15" spans="1:23" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>13</v>
       </c>
@@ -4854,7 +4930,7 @@
       <c r="T15" s="10"/>
       <c r="W15" s="10"/>
     </row>
-    <row r="16" spans="1:23" ht="45">
+    <row r="16" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>14</v>
       </c>
@@ -4875,7 +4951,7 @@
       <c r="T16" s="10"/>
       <c r="W16" s="10"/>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>15</v>
       </c>
@@ -4894,7 +4970,7 @@
       <c r="U17" s="1"/>
       <c r="W17" s="10"/>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>16</v>
       </c>
@@ -4913,7 +4989,7 @@
       <c r="U18" s="1"/>
       <c r="W18" s="10"/>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>17</v>
       </c>
@@ -4932,7 +5008,7 @@
       <c r="U19" s="1"/>
       <c r="W19" s="10"/>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>18</v>
       </c>
@@ -4951,7 +5027,7 @@
       <c r="U20" s="1"/>
       <c r="W20" s="10"/>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>19</v>
       </c>
@@ -4970,7 +5046,7 @@
       <c r="U21" s="1"/>
       <c r="W21" s="10"/>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>20</v>
       </c>
@@ -4989,7 +5065,7 @@
       <c r="U22" s="1"/>
       <c r="W22" s="10"/>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>21</v>
       </c>
@@ -5008,7 +5084,7 @@
       <c r="U23" s="1"/>
       <c r="W23" s="10"/>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>22</v>
       </c>
@@ -5026,7 +5102,7 @@
       <c r="T24" s="10"/>
       <c r="W24" s="10"/>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>23</v>
       </c>
@@ -5045,7 +5121,7 @@
       <c r="U25" s="1"/>
       <c r="W25" s="10"/>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>31</v>
       </c>
@@ -5064,7 +5140,7 @@
       <c r="U26" s="1"/>
       <c r="W26" s="10"/>
     </row>
-    <row r="27" spans="1:23" ht="30">
+    <row r="27" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>32</v>
       </c>
@@ -5086,7 +5162,7 @@
       <c r="U27" s="1"/>
       <c r="W27" s="10"/>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>34</v>
       </c>
@@ -5105,7 +5181,7 @@
       <c r="U28" s="1"/>
       <c r="W28" s="10"/>
     </row>
-    <row r="29" spans="1:23" ht="30">
+    <row r="29" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>36</v>
       </c>
@@ -5127,7 +5203,7 @@
       <c r="U29" s="1"/>
       <c r="W29" s="10"/>
     </row>
-    <row r="30" spans="1:23" ht="30">
+    <row r="30" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>38</v>
       </c>
@@ -5147,7 +5223,7 @@
       <c r="U30" s="1"/>
       <c r="W30" s="10"/>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>24</v>
       </c>
@@ -5166,7 +5242,7 @@
       <c r="U31" s="1"/>
       <c r="W31" s="10"/>
     </row>
-    <row r="32" spans="1:23" ht="15.75" thickBot="1">
+    <row r="32" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="20"/>
       <c r="B32" s="15"/>
       <c r="C32" s="16"/>
@@ -5202,4 +5278,416 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="50.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="66" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="67"/>
+      <c r="E1" s="68"/>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="74"/>
+      <c r="E3" s="71"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="74"/>
+      <c r="E4" s="71"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="74"/>
+      <c r="E5" s="71"/>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="74"/>
+      <c r="E6" s="71"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>5</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="74"/>
+      <c r="E7" s="71"/>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="E8" s="71"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="74"/>
+      <c r="E9" s="71"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="74"/>
+      <c r="E10" s="71"/>
+    </row>
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>9</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="74"/>
+      <c r="E11" s="71"/>
+    </row>
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>10</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="74"/>
+      <c r="E12" s="71"/>
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>11</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="E13" s="71" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>12</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="74"/>
+      <c r="E14" s="71"/>
+    </row>
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="74"/>
+      <c r="E15" s="71"/>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>14</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="76" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" s="74" t="s">
+        <v>149</v>
+      </c>
+      <c r="E16" s="71"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>15</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="74"/>
+      <c r="E17" s="71"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>16</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="70"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="71"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>17</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="70"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="71"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="70"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="71"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>19</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="70"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="71"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>20</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="70"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="71"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>21</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="70"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="71"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>22</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="70"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="71"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>23</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="70"/>
+      <c r="D25" s="74"/>
+      <c r="E25" s="71"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="70"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="71"/>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="70"/>
+      <c r="D27" s="74"/>
+      <c r="E27" s="71"/>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="70"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="71"/>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="70"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="71"/>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="70"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="71"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="20">
+        <v>24</v>
+      </c>
+      <c r="B31" s="69" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="72"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="73"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>